<commit_message>
Mathieu + Abdo Check
</commit_message>
<xml_diff>
--- a/Assignment 1/EGI_Assignment1_NuurVdVelGrotz.xlsx
+++ b/Assignment 1/EGI_Assignment1_NuurVdVelGrotz.xlsx
@@ -861,7 +861,7 @@
         <v>2040</v>
       </c>
       <c r="B22">
-        <v>81.99500000000001</v>
+        <v>81.995</v>
       </c>
       <c r="C22">
         <v>4978254.674</v>
@@ -1356,7 +1356,7 @@
         <v>0.021</v>
       </c>
       <c r="F43">
-        <v>6135512.963000001</v>
+        <v>6135512.963</v>
       </c>
       <c r="G43">
         <v>39852.553</v>
@@ -1934,7 +1934,7 @@
         <v>21691260.997</v>
       </c>
       <c r="G68">
-        <v>66553.241</v>
+        <v>66553.24099999999</v>
       </c>
     </row>
     <row r="69">
@@ -2426,7 +2426,7 @@
         <v>0.05</v>
       </c>
       <c r="H5">
-        <v>768310.945</v>
+        <v>768310.9449999999</v>
       </c>
       <c r="I5">
         <v>15604.074</v>
@@ -2542,7 +2542,7 @@
         <v>0.05</v>
       </c>
       <c r="H9">
-        <v>975564.1530000001</v>
+        <v>975564.153</v>
       </c>
       <c r="I9">
         <v>17572.821</v>
@@ -2904,7 +2904,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>81.99500000000001</v>
+        <v>81.995</v>
       </c>
       <c r="D22">
         <v>4867816.202</v>
@@ -4618,7 +4618,7 @@
         <v>481.383</v>
       </c>
       <c r="D81">
-        <v>97322292.84800001</v>
+        <v>97322292.848</v>
       </c>
       <c r="E81">
         <v>43275.701</v>
@@ -5245,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>81.99500000000001</v>
+        <v>81.995</v>
       </c>
       <c r="D22">
         <v>4918103.455</v>
@@ -6638,7 +6638,7 @@
         <v>26684347.931</v>
       </c>
       <c r="H75">
-        <v>66365.01</v>
+        <v>66365.00999999999</v>
       </c>
     </row>
     <row r="76">
@@ -6820,7 +6820,7 @@
         <v>36427192.582</v>
       </c>
       <c r="H82">
-        <v>73435.563</v>
+        <v>73435.56299999999</v>
       </c>
     </row>
   </sheetData>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Y_sim2</t>
+          <t>Y_sim3</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -7465,7 +7465,7 @@
         <v>2040</v>
       </c>
       <c r="B22">
-        <v>81.99500000000001</v>
+        <v>81.995</v>
       </c>
       <c r="C22">
         <v>4797125.296</v>
@@ -8037,7 +8037,7 @@
         <v>30293.545</v>
       </c>
       <c r="I41">
-        <v>4392251.088000001</v>
+        <v>4392251.088</v>
       </c>
     </row>
     <row r="42">
@@ -9275,7 +9275,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Y_sim2</t>
+          <t>Y_sim3</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -9874,7 +9874,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>81.99500000000001</v>
+        <v>81.995</v>
       </c>
       <c r="D22">
         <v>4918103.455</v>
@@ -11743,19 +11743,19 @@
         <v>634165.406</v>
       </c>
       <c r="J2">
-        <v>634165.4060852079</v>
+        <v>634165.406</v>
       </c>
       <c r="K2">
-        <v>14092.56457967129</v>
+        <v>14092.565</v>
       </c>
       <c r="L2">
-        <v>462940.7464422018</v>
+        <v>462940.746</v>
       </c>
       <c r="M2">
-        <v>475624.0545</v>
+        <v>475624.054</v>
       </c>
       <c r="N2">
-        <v>0.9733333334641127</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="3">
@@ -11766,40 +11766,40 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>46.37045402790826</v>
+        <v>46.37</v>
       </c>
       <c r="D3">
-        <v>1191304.791521302</v>
+        <v>1191304.792</v>
       </c>
       <c r="E3">
-        <v>11082.18190436224</v>
+        <v>11082.182</v>
       </c>
       <c r="F3">
-        <v>0.03785530250857538</v>
+        <v>0.038</v>
       </c>
       <c r="G3">
-        <v>12683.30812170416</v>
+        <v>12683.308</v>
       </c>
       <c r="H3">
         <v>678216.249</v>
       </c>
       <c r="I3">
-        <v>0.04559195764938849</v>
+        <v>0.046</v>
       </c>
       <c r="J3">
-        <v>678216.2487433798</v>
+        <v>678216.249</v>
       </c>
       <c r="K3">
-        <v>14626.04287495638</v>
+        <v>14626.043</v>
       </c>
       <c r="L3">
-        <v>495097.8615826673</v>
+        <v>495097.862</v>
       </c>
       <c r="M3">
-        <v>508662.18675</v>
+        <v>508662.187</v>
       </c>
       <c r="N3">
-        <v>0.9733333329650482</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="4">
@@ -11810,40 +11810,40 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>47.78264459454118</v>
+        <v>47.783</v>
       </c>
       <c r="D4">
-        <v>1313206.662046295</v>
+        <v>1313206.662</v>
       </c>
       <c r="E4">
-        <v>11306.05682925062</v>
+        <v>11306.057</v>
       </c>
       <c r="F4">
-        <v>0.03629259052955153</v>
+        <v>0.036</v>
       </c>
       <c r="G4">
-        <v>25740.30077170359</v>
+        <v>25740.301</v>
       </c>
       <c r="H4">
         <v>724234.848</v>
       </c>
       <c r="I4">
-        <v>0.0417093632839791</v>
+        <v>0.042</v>
       </c>
       <c r="J4">
-        <v>724234.8478637008</v>
+        <v>724234.848</v>
       </c>
       <c r="K4">
-        <v>15156.85986008484</v>
+        <v>15156.86</v>
       </c>
       <c r="L4">
-        <v>528691.4389405015</v>
+        <v>528691.439</v>
       </c>
       <c r="M4">
-        <v>543176.1359999999</v>
+        <v>543176.1360000001</v>
       </c>
       <c r="N4">
-        <v>0.9733333331501545</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="5">
@@ -11854,40 +11854,40 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>49.23784276673447</v>
+        <v>49.238</v>
       </c>
       <c r="D5">
-        <v>1441737.107530368</v>
+        <v>1441737.108</v>
       </c>
       <c r="E5">
-        <v>11534.45432762014</v>
+        <v>11534.454</v>
       </c>
       <c r="F5">
-        <v>0.03490984990584719</v>
+        <v>0.035</v>
       </c>
       <c r="G5">
-        <v>39195.38569810947</v>
+        <v>39195.386</v>
       </c>
       <c r="H5">
         <v>772343.992</v>
       </c>
       <c r="I5">
-        <v>0.03828137478027435</v>
+        <v>0.038</v>
       </c>
       <c r="J5">
-        <v>772343.9923089118</v>
+        <v>772343.992</v>
       </c>
       <c r="K5">
-        <v>15685.98356284436</v>
+        <v>15685.984</v>
       </c>
       <c r="L5">
-        <v>563811.1143855056</v>
+        <v>563811.1139999999</v>
       </c>
       <c r="M5">
-        <v>579257.994</v>
+        <v>579257.9939999999</v>
       </c>
       <c r="N5">
-        <v>0.9733333337226342</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="6">
@@ -11898,40 +11898,40 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>50.73735832107191</v>
+        <v>50.737</v>
       </c>
       <c r="D6">
-        <v>1577153.621306381</v>
+        <v>1577153.621</v>
       </c>
       <c r="E6">
-        <v>11767.46576151548</v>
+        <v>11767.466</v>
       </c>
       <c r="F6">
-        <v>0.03367983608778361</v>
+        <v>0.034</v>
       </c>
       <c r="G6">
-        <v>53074.45011636333</v>
+        <v>53074.45</v>
       </c>
       <c r="H6">
         <v>822669.9840000001</v>
       </c>
       <c r="I6">
-        <v>0.03524785203659365</v>
+        <v>0.035</v>
       </c>
       <c r="J6">
-        <v>822669.9838104352</v>
+        <v>822669.9840000001</v>
       </c>
       <c r="K6">
-        <v>16214.28491811662</v>
+        <v>16214.285</v>
       </c>
       <c r="L6">
-        <v>600549.0881816177</v>
+        <v>600549.088</v>
       </c>
       <c r="M6">
         <v>617002.488</v>
       </c>
       <c r="N6">
-        <v>0.9733333331090517</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="7">
@@ -11942,40 +11942,40 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>52.28254092277274</v>
+        <v>52.283</v>
       </c>
       <c r="D7">
-        <v>1719734.972406735</v>
+        <v>1719734.972</v>
       </c>
       <c r="E7">
-        <v>12005.18433861706</v>
+        <v>12005.184</v>
       </c>
       <c r="F7">
-        <v>0.03258048787045819</v>
+        <v>0.033</v>
       </c>
       <c r="G7">
-        <v>67404.8717879175</v>
+        <v>67404.872</v>
       </c>
       <c r="H7">
         <v>875343.277</v>
       </c>
       <c r="I7">
-        <v>0.03255760858478596</v>
+        <v>0.033</v>
       </c>
       <c r="J7">
-        <v>875343.2767454741</v>
+        <v>875343.277</v>
       </c>
       <c r="K7">
-        <v>16742.55423121947</v>
+        <v>16742.554</v>
       </c>
       <c r="L7">
-        <v>639000.5920241961</v>
+        <v>639000.5919999999</v>
       </c>
       <c r="M7">
-        <v>656507.4577500001</v>
+        <v>656507.458</v>
       </c>
       <c r="N7">
-        <v>0.9733333330503144</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="8">
@@ -11986,40 +11986,40 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>53.87478134048146</v>
+        <v>53.875</v>
       </c>
       <c r="D8">
-        <v>1869781.392696834</v>
+        <v>1869781.393</v>
       </c>
       <c r="E8">
-        <v>12247.70514952534</v>
+        <v>12247.705</v>
       </c>
       <c r="F8">
-        <v>0.03159375203991938</v>
+        <v>0.032</v>
       </c>
       <c r="G8">
-        <v>82215.54245131028</v>
+        <v>82215.542</v>
       </c>
       <c r="H8">
         <v>930499.058</v>
       </c>
       <c r="I8">
-        <v>0.03016696361859184</v>
+        <v>0.03</v>
       </c>
       <c r="J8">
-        <v>930499.0583849642</v>
+        <v>930499.058</v>
       </c>
       <c r="K8">
-        <v>17271.51433811553</v>
+        <v>17271.514</v>
       </c>
       <c r="L8">
-        <v>679264.3126210239</v>
+        <v>679264.313</v>
       </c>
       <c r="M8">
-        <v>697874.2934999999</v>
+        <v>697874.2929999999</v>
       </c>
       <c r="N8">
-        <v>0.9733333337360189</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="9">
@@ -12030,40 +12030,40 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>55.51551269805344</v>
+        <v>55.516</v>
       </c>
       <c r="D9">
-        <v>2027614.901585201</v>
+        <v>2027614.902</v>
       </c>
       <c r="E9">
-        <v>12495.12520579835</v>
+        <v>12495.125</v>
       </c>
       <c r="F9">
-        <v>0.03070471357176544</v>
+        <v>0.031</v>
       </c>
       <c r="G9">
-        <v>97536.90192095714</v>
+        <v>97536.902</v>
       </c>
       <c r="H9">
         <v>988277.7879999999</v>
       </c>
       <c r="I9">
-        <v>0.0280385414244155</v>
+        <v>0.028</v>
       </c>
       <c r="J9">
-        <v>988277.7881872052</v>
+        <v>988277.7879999999</v>
       </c>
       <c r="K9">
-        <v>17801.831238818</v>
+        <v>17801.831</v>
       </c>
       <c r="L9">
-        <v>721442.7853766598</v>
+        <v>721442.785</v>
       </c>
       <c r="M9">
         <v>741208.341</v>
       </c>
       <c r="N9">
-        <v>0.9733333335177077</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="10">
@@ -12074,40 +12074,40 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>57.20621176446321</v>
+        <v>57.206</v>
       </c>
       <c r="D10">
-        <v>2193579.752568595</v>
+        <v>2193579.753</v>
       </c>
       <c r="E10">
-        <v>12747.54347875757</v>
+        <v>12747.543</v>
       </c>
       <c r="F10">
-        <v>0.02990094267432323</v>
+        <v>0.03</v>
       </c>
       <c r="G10">
-        <v>113400.981607863</v>
+        <v>113400.982</v>
       </c>
       <c r="H10">
         <v>1048825.71</v>
       </c>
       <c r="I10">
-        <v>0.02614027445099734</v>
+        <v>0.026</v>
       </c>
       <c r="J10">
-        <v>1048825.709935859</v>
+        <v>1048825.71</v>
       </c>
       <c r="K10">
-        <v>18334.12277418788</v>
+        <v>18334.123</v>
       </c>
       <c r="L10">
-        <v>765642.7682531773</v>
+        <v>765642.768</v>
       </c>
       <c r="M10">
-        <v>786619.2825</v>
+        <v>786619.282</v>
       </c>
       <c r="N10">
-        <v>0.9733333332738093</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="11">
@@ -12118,40 +12118,40 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>58.94840028299613</v>
+        <v>58.948</v>
       </c>
       <c r="D11">
-        <v>2368042.989949815</v>
+        <v>2368042.99</v>
       </c>
       <c r="E11">
-        <v>13005.06093907781</v>
+        <v>13005.061</v>
       </c>
       <c r="F11">
-        <v>0.0291719981982464</v>
+        <v>0.029</v>
       </c>
       <c r="G11">
-        <v>129841.4565422656</v>
+        <v>129841.457</v>
       </c>
       <c r="H11">
         <v>1112295.347</v>
       </c>
       <c r="I11">
-        <v>0.02444457403455489</v>
+        <v>0.024</v>
       </c>
       <c r="J11">
-        <v>1112295.347178727</v>
+        <v>1112295.347</v>
       </c>
       <c r="K11">
-        <v>18868.96577072291</v>
+        <v>18868.966</v>
       </c>
       <c r="L11">
-        <v>811975.6034404704</v>
+        <v>811975.603</v>
       </c>
       <c r="M11">
-        <v>834221.5102500001</v>
+        <v>834221.51</v>
       </c>
       <c r="N11">
-        <v>0.9733333334897311</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="12">
@@ -12162,40 +12162,40 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>60.74364634092014</v>
+        <v>60.744</v>
       </c>
       <c r="D12">
-        <v>2551395.107146505</v>
+        <v>2551395.107</v>
       </c>
       <c r="E12">
-        <v>13267.7805971768</v>
+        <v>13267.781</v>
       </c>
       <c r="F12">
-        <v>0.0285090454530711</v>
+        <v>0.029</v>
       </c>
       <c r="G12">
-        <v>146893.7052241495</v>
+        <v>146893.705</v>
       </c>
       <c r="H12">
         <v>1178845.99</v>
       </c>
       <c r="I12">
-        <v>0.02292763926275244</v>
+        <v>0.023</v>
       </c>
       <c r="J12">
-        <v>1178845.990053187</v>
+        <v>1178845.99</v>
       </c>
       <c r="K12">
-        <v>19406.9019735329</v>
+        <v>19406.902</v>
       </c>
       <c r="L12">
-        <v>860557.5727388267</v>
+        <v>860557.573</v>
       </c>
       <c r="M12">
-        <v>884134.4924999999</v>
+        <v>884134.492</v>
       </c>
       <c r="N12">
-        <v>0.9733333333772484</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="13">
@@ -12206,40 +12206,40 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>62.59356578087012</v>
+        <v>62.594</v>
       </c>
       <c r="D13">
-        <v>2744050.800373942</v>
+        <v>2744050.8</v>
       </c>
       <c r="E13">
-        <v>13535.80754442076</v>
+        <v>13535.808</v>
       </c>
       <c r="F13">
-        <v>0.02790455885126761</v>
+        <v>0.028</v>
       </c>
       <c r="G13">
-        <v>164594.8768162473</v>
+        <v>164594.877</v>
       </c>
       <c r="H13">
         <v>1248644.18</v>
       </c>
       <c r="I13">
-        <v>0.02156887979457669</v>
+        <v>0.022</v>
       </c>
       <c r="J13">
-        <v>1248644.179883422</v>
+        <v>1248644.18</v>
       </c>
       <c r="K13">
-        <v>19948.44301177413</v>
+        <v>19948.443</v>
       </c>
       <c r="L13">
-        <v>911510.2513148983</v>
+        <v>911510.251</v>
       </c>
       <c r="M13">
         <v>936483.135</v>
       </c>
       <c r="N13">
-        <v>0.9733333332424595</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="14">
@@ -12250,40 +12250,40 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>64.49982365521531</v>
+        <v>64.5</v>
       </c>
       <c r="D14">
-        <v>2946449.81332984</v>
+        <v>2946449.813</v>
       </c>
       <c r="E14">
-        <v>13809.24899516233</v>
+        <v>13809.249</v>
       </c>
       <c r="F14">
-        <v>0.02735208822065411</v>
+        <v>0.027</v>
       </c>
       <c r="G14">
-        <v>182983.9653412658</v>
+        <v>182983.965</v>
       </c>
       <c r="H14">
         <v>1321864.197</v>
       </c>
       <c r="I14">
-        <v>0.02035043283009756</v>
+        <v>0.02</v>
       </c>
       <c r="J14">
-        <v>1321864.196702678</v>
+        <v>1321864.197</v>
       </c>
       <c r="K14">
-        <v>20494.07458489686</v>
+        <v>20494.075</v>
       </c>
       <c r="L14">
-        <v>964960.8635929546</v>
+        <v>964960.8639999999</v>
       </c>
       <c r="M14">
-        <v>991398.14775</v>
+        <v>991398.148</v>
       </c>
       <c r="N14">
-        <v>0.9733333331144047</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="15">
@@ -12294,40 +12294,40 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>66.46413572471892</v>
+        <v>66.464</v>
       </c>
       <c r="D15">
-        <v>3159057.869972315</v>
+        <v>3159057.87</v>
       </c>
       <c r="E15">
-        <v>14088.21432962774</v>
+        <v>14088.214</v>
       </c>
       <c r="F15">
-        <v>0.02684607344456283</v>
+        <v>0.027</v>
       </c>
       <c r="G15">
-        <v>202101.8906616687</v>
+        <v>202101.891</v>
       </c>
       <c r="H15">
         <v>1398688.554</v>
       </c>
       <c r="I15">
-        <v>0.01925675800424624</v>
+        <v>0.019</v>
       </c>
       <c r="J15">
-        <v>1398688.553955046</v>
+        <v>1398688.554</v>
       </c>
       <c r="K15">
-        <v>21044.26001638135</v>
+        <v>21044.26</v>
       </c>
       <c r="L15">
-        <v>1021042.644387183</v>
+        <v>1021042.644</v>
       </c>
       <c r="M15">
-        <v>1049016.4155</v>
+        <v>1049016.416</v>
       </c>
       <c r="N15">
-        <v>0.9733333333020499</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="16">
@@ -12338,40 +12338,40 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>68.48827000283852</v>
+        <v>68.488</v>
       </c>
       <c r="D16">
-        <v>3382367.693662183</v>
+        <v>3382367.694</v>
       </c>
       <c r="E16">
-        <v>14372.81513767036</v>
+        <v>14372.815</v>
       </c>
       <c r="F16">
-        <v>0.02638169616890608</v>
+        <v>0.026</v>
       </c>
       <c r="G16">
-        <v>221991.5861143029</v>
+        <v>221991.586</v>
       </c>
       <c r="H16">
         <v>1479308.504</v>
       </c>
       <c r="I16">
-        <v>0.01827429690158997</v>
+        <v>0.018</v>
       </c>
       <c r="J16">
-        <v>1479308.503972475</v>
+        <v>1479308.504</v>
       </c>
       <c r="K16">
-        <v>21599.44329023298</v>
+        <v>21599.443</v>
       </c>
       <c r="L16">
-        <v>1079895.207899907</v>
+        <v>1079895.208</v>
       </c>
       <c r="M16">
         <v>1109481.378</v>
       </c>
       <c r="N16">
-        <v>0.9733333333152232</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="17">
@@ -12382,40 +12382,40 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>70.5740483470576</v>
+        <v>70.574</v>
       </c>
       <c r="D17">
-        <v>3616900.111908815</v>
+        <v>3616900.112</v>
       </c>
       <c r="E17">
-        <v>14663.16526340814</v>
+        <v>14663.165</v>
       </c>
       <c r="F17">
-        <v>0.02595476021463725</v>
+        <v>0.026</v>
       </c>
       <c r="G17">
-        <v>242698.0927491803</v>
+        <v>242698.093</v>
       </c>
       <c r="H17">
         <v>1563924.557</v>
       </c>
       <c r="I17">
-        <v>0.0173911862730208</v>
+        <v>0.017</v>
       </c>
       <c r="J17">
-        <v>1563924.557339097</v>
+        <v>1563924.557</v>
       </c>
       <c r="K17">
-        <v>22160.05166160064</v>
+        <v>22160.052</v>
       </c>
       <c r="L17">
-        <v>1141664.926857541</v>
+        <v>1141664.927</v>
       </c>
       <c r="M17">
-        <v>1172943.41775</v>
+        <v>1172943.418</v>
       </c>
       <c r="N17">
-        <v>0.973333333544376</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="18">
@@ -12426,40 +12426,40 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>72.72334809868021</v>
+        <v>72.723</v>
       </c>
       <c r="D18">
-        <v>3863205.246767237</v>
+        <v>3863205.247</v>
       </c>
       <c r="E18">
-        <v>14711.09976774404</v>
+        <v>14711.1</v>
       </c>
       <c r="F18">
-        <v>0.01412588611094469</v>
+        <v>0.014</v>
       </c>
       <c r="G18">
-        <v>264268.660185995</v>
+        <v>264268.66</v>
       </c>
       <c r="H18">
         <v>1596912.785</v>
       </c>
       <c r="I18">
-        <v>0.01659701597917845</v>
+        <v>0.017</v>
       </c>
       <c r="J18">
-        <v>1634317.767142262</v>
+        <v>1634317.767</v>
       </c>
       <c r="K18">
-        <v>22473.08202758506</v>
+        <v>22473.082</v>
       </c>
       <c r="L18">
-        <v>1193051.970013851</v>
+        <v>1193051.97</v>
       </c>
       <c r="M18">
-        <v>1197684.58875</v>
+        <v>1197684.589</v>
       </c>
       <c r="N18">
-        <v>0.996132021084964</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="19">
@@ -12470,40 +12470,40 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>74.93810377256489</v>
+        <v>74.938</v>
       </c>
       <c r="D19">
-        <v>4117256.478682113</v>
+        <v>4117256.479</v>
       </c>
       <c r="E19">
-        <v>15008.28369631976</v>
+        <v>15008.284</v>
       </c>
       <c r="F19">
-        <v>0.02482067095506533</v>
+        <v>0.025</v>
       </c>
       <c r="G19">
-        <v>286384.2691214004</v>
+        <v>286384.269</v>
       </c>
       <c r="H19">
         <v>1685124.653</v>
       </c>
       <c r="I19">
-        <v>0.01570964637220605</v>
+        <v>0.016</v>
       </c>
       <c r="J19">
-        <v>1725890.400620611</v>
+        <v>1725890.401</v>
       </c>
       <c r="K19">
-        <v>23030.87900193794</v>
+        <v>23030.879</v>
       </c>
       <c r="L19">
-        <v>1259899.992453046</v>
+        <v>1259899.992</v>
       </c>
       <c r="M19">
-        <v>1263843.48975</v>
+        <v>1263843.49</v>
       </c>
       <c r="N19">
-        <v>0.9968797581908389</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="20">
@@ -12514,40 +12514,40 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>77.22030879831864</v>
+        <v>77.22</v>
       </c>
       <c r="D20">
-        <v>4384038.819689981</v>
+        <v>4384038.82</v>
       </c>
       <c r="E20">
-        <v>15311.47113848714</v>
+        <v>15311.471</v>
       </c>
       <c r="F20">
-        <v>0.02451416087141255</v>
+        <v>0.025</v>
       </c>
       <c r="G20">
-        <v>309446.7063689567</v>
+        <v>309446.706</v>
       </c>
       <c r="H20">
         <v>1777774.612</v>
       </c>
       <c r="I20">
-        <v>0.01508878986668883</v>
+        <v>0.015</v>
       </c>
       <c r="J20">
-        <v>1822048.836767063</v>
+        <v>1822048.837</v>
       </c>
       <c r="K20">
-        <v>23595.46167480148</v>
+        <v>23595.462</v>
       </c>
       <c r="L20">
-        <v>1330095.650839956</v>
+        <v>1330095.651</v>
       </c>
       <c r="M20">
         <v>1333330.959</v>
       </c>
       <c r="N20">
-        <v>0.9975735145590032</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="21">
@@ -12558,40 +12558,40 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>79.57201731451808</v>
+        <v>79.572</v>
       </c>
       <c r="D21">
-        <v>4664189.476094147</v>
+        <v>4664189.476</v>
       </c>
       <c r="E21">
-        <v>15620.78337326557</v>
+        <v>15620.783</v>
       </c>
       <c r="F21">
-        <v>0.02423030726584812</v>
+        <v>0.024</v>
       </c>
       <c r="G21">
-        <v>333509.8148495397</v>
+        <v>333509.815</v>
       </c>
       <c r="H21">
         <v>1875092.735</v>
       </c>
       <c r="I21">
-        <v>0.01452994509976338</v>
+        <v>0.015</v>
       </c>
       <c r="J21">
-        <v>1923031.819324693</v>
+        <v>1923031.819</v>
       </c>
       <c r="K21">
-        <v>24167.18696126147</v>
+        <v>24167.187</v>
       </c>
       <c r="L21">
-        <v>1403813.228107026</v>
+        <v>1403813.228</v>
       </c>
       <c r="M21">
-        <v>1406319.55125</v>
+        <v>1406319.551</v>
       </c>
       <c r="N21">
-        <v>0.9982178139095438</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="22">
@@ -12602,40 +12602,40 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>81.9953460175729</v>
+        <v>81.995</v>
       </c>
       <c r="D22">
-        <v>4958379.851881554</v>
+        <v>4958379.852</v>
       </c>
       <c r="E22">
-        <v>15936.3441296732</v>
+        <v>15936.344</v>
       </c>
       <c r="F22">
-        <v>0.02396714432335344</v>
+        <v>0.024</v>
       </c>
       <c r="G22">
-        <v>358630.0586420519</v>
+        <v>358630.059</v>
       </c>
       <c r="H22">
         <v>1977320.725</v>
       </c>
       <c r="I22">
-        <v>0.01402702347301568</v>
+        <v>0.014</v>
       </c>
       <c r="J22">
-        <v>2029090.075026267</v>
+        <v>2029090.075</v>
       </c>
       <c r="K22">
-        <v>24746.40541905148</v>
+        <v>24746.405</v>
       </c>
       <c r="L22">
-        <v>1481235.754769175</v>
+        <v>1481235.755</v>
       </c>
       <c r="M22">
-        <v>1482990.54375</v>
+        <v>1482990.544</v>
       </c>
       <c r="N22">
-        <v>0.9988167227443084</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="23">
@@ -12646,40 +12646,40 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>84.49247606689545</v>
+        <v>84.492</v>
       </c>
       <c r="D23">
-        <v>5267317.176562859</v>
+        <v>5267317.177</v>
       </c>
       <c r="E23">
-        <v>16258.27963622012</v>
+        <v>16258.28</v>
       </c>
       <c r="F23">
-        <v>0.02372291328846522</v>
+        <v>0.024</v>
       </c>
       <c r="G23">
-        <v>384866.6577968952</v>
+        <v>384866.658</v>
       </c>
       <c r="H23">
         <v>2084712.525</v>
       </c>
       <c r="I23">
-        <v>0.01357460502104279</v>
+        <v>0.014</v>
       </c>
       <c r="J23">
-        <v>2140486.952765979</v>
+        <v>2140486.953</v>
       </c>
       <c r="K23">
-        <v>25333.46224900885</v>
+        <v>25333.462</v>
       </c>
       <c r="L23">
-        <v>1562555.475519165</v>
+        <v>1562555.476</v>
       </c>
       <c r="M23">
-        <v>1563534.39375</v>
+        <v>1563534.394</v>
       </c>
       <c r="N23">
-        <v>0.9993739068134683</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="24">
@@ -12690,40 +12690,40 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>87.06565504809142</v>
+        <v>87.066</v>
       </c>
       <c r="D24">
-        <v>5591746.227691839</v>
+        <v>5591746.228</v>
       </c>
       <c r="E24">
-        <v>16586.71867140149</v>
+        <v>16586.719</v>
       </c>
       <c r="F24">
-        <v>0.02349603609867981</v>
+        <v>0.023</v>
       </c>
       <c r="G24">
-        <v>412281.730540339</v>
+        <v>412281.731</v>
       </c>
       <c r="H24">
         <v>2197534.961</v>
       </c>
       <c r="I24">
-        <v>0.01316785010214127</v>
+        <v>0.013</v>
       </c>
       <c r="J24">
-        <v>2257499.092675678</v>
+        <v>2257499.093</v>
       </c>
       <c r="K24">
-        <v>25928.6981925161</v>
+        <v>25928.698</v>
       </c>
       <c r="L24">
-        <v>1647974.337653245</v>
+        <v>1647974.338</v>
       </c>
       <c r="M24">
-        <v>1648151.22075</v>
+        <v>1648151.221</v>
       </c>
       <c r="N24">
-        <v>0.9998926778717099</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -12734,40 +12734,40 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>89.7171989959387</v>
+        <v>89.717</v>
       </c>
       <c r="D25">
-        <v>5932451.151753085</v>
+        <v>5932451.152</v>
       </c>
       <c r="E25">
-        <v>16921.79261521061</v>
+        <v>16921.793</v>
       </c>
       <c r="F25">
-        <v>0.02328509296084497</v>
+        <v>0.023</v>
       </c>
       <c r="G25">
-        <v>440940.443172239</v>
+        <v>440940.443</v>
       </c>
       <c r="H25">
         <v>2316068.412</v>
       </c>
       <c r="I25">
-        <v>0.01280242410849337</v>
+        <v>0.013</v>
       </c>
       <c r="J25">
-        <v>2380417.12702899</v>
+        <v>2380417.127</v>
       </c>
       <c r="K25">
-        <v>26532.45034028253</v>
+        <v>26532.45</v>
       </c>
       <c r="L25">
-        <v>1737704.502731162</v>
+        <v>1737704.503</v>
       </c>
       <c r="M25">
         <v>1737051.309</v>
       </c>
       <c r="N25">
-        <v>1.000376035945385</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -12778,40 +12778,40 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>92.44949447897494</v>
+        <v>92.449</v>
       </c>
       <c r="D26">
-        <v>6290257.387440208</v>
+        <v>6290257.387</v>
       </c>
       <c r="E26">
-        <v>17263.63550169272</v>
+        <v>17263.636</v>
       </c>
       <c r="F26">
-        <v>0.02308880319857711</v>
+        <v>0.023</v>
       </c>
       <c r="G26">
-        <v>470911.1679859292</v>
+        <v>470911.168</v>
       </c>
       <c r="H26">
         <v>2440607.516</v>
       </c>
       <c r="I26">
-        <v>0.01247443319571369</v>
+        <v>0.012</v>
       </c>
       <c r="J26">
-        <v>2509546.414934116</v>
+        <v>2509546.415</v>
       </c>
       <c r="K26">
-        <v>27145.05286456534</v>
+        <v>27145.053</v>
       </c>
       <c r="L26">
-        <v>1831968.882901905</v>
+        <v>1831968.883</v>
       </c>
       <c r="M26">
         <v>1830455.637</v>
       </c>
       <c r="N26">
-        <v>1.000826704494398</v>
+        <v>1.001</v>
       </c>
     </row>
     <row r="27">
@@ -12822,40 +12822,40 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>95.26500074757037</v>
+        <v>95.265</v>
       </c>
       <c r="D27">
-        <v>6666033.695676129</v>
+        <v>6666033.696</v>
       </c>
       <c r="E27">
-        <v>17612.38407256039</v>
+        <v>17612.384</v>
       </c>
       <c r="F27">
-        <v>0.02290600882641763</v>
+        <v>0.023</v>
       </c>
       <c r="G27">
-        <v>502265.6495651744</v>
+        <v>502265.65</v>
       </c>
       <c r="H27">
         <v>2571461.914</v>
       </c>
       <c r="I27">
-        <v>0.01218036935847268</v>
+        <v>0.012</v>
       </c>
       <c r="J27">
-        <v>2645207.812826301</v>
+        <v>2645207.813</v>
       </c>
       <c r="K27">
-        <v>27766.83768507464</v>
+        <v>27766.838</v>
       </c>
       <c r="L27">
-        <v>1931001.7033632</v>
+        <v>1931001.703</v>
       </c>
       <c r="M27">
-        <v>1928596.4355</v>
+        <v>1928596.435</v>
       </c>
       <c r="N27">
-        <v>1.0012471597577</v>
+        <v>1.001</v>
       </c>
     </row>
     <row r="28">
@@ -12866,40 +12866,40 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>98.16625194741904</v>
+        <v>98.166</v>
       </c>
       <c r="D28">
-        <v>7060694.30105566</v>
+        <v>7060694.301</v>
       </c>
       <c r="E28">
-        <v>17968.177831892</v>
+        <v>17968.178</v>
       </c>
       <c r="F28">
-        <v>0.02273566040747011</v>
+        <v>0.023</v>
       </c>
       <c r="G28">
-        <v>535079.1798390934</v>
+        <v>535079.1800000001</v>
       </c>
       <c r="H28">
         <v>2708957.023</v>
       </c>
       <c r="I28">
-        <v>0.01191706344773102</v>
+        <v>0.012</v>
       </c>
       <c r="J28">
-        <v>2787738.482832306</v>
+        <v>2787738.483</v>
       </c>
       <c r="K28">
-        <v>28398.13507727184</v>
+        <v>28398.135</v>
       </c>
       <c r="L28">
-        <v>2035049.092467584</v>
+        <v>2035049.092</v>
       </c>
       <c r="M28">
-        <v>2031717.76725</v>
+        <v>2031717.767</v>
       </c>
       <c r="N28">
-        <v>1.00163965944054</v>
+        <v>1.002</v>
       </c>
     </row>
     <row r="29">
@@ -12910,40 +12910,40 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>101.1558594004412</v>
+        <v>101.156</v>
       </c>
       <c r="D29">
-        <v>7475201.149721509</v>
+        <v>7475201.15</v>
       </c>
       <c r="E29">
-        <v>18117.02100984449</v>
+        <v>18117.021</v>
       </c>
       <c r="F29">
-        <v>0.01455789402003806</v>
+        <v>0.015</v>
       </c>
       <c r="G29">
-        <v>569430.7823021758</v>
+        <v>569430.782</v>
       </c>
       <c r="H29">
         <v>2757038.163</v>
       </c>
       <c r="I29">
-        <v>0.01168164494672731</v>
+        <v>0.012</v>
       </c>
       <c r="J29">
-        <v>2914457.315166349</v>
+        <v>2914457.315</v>
       </c>
       <c r="K29">
-        <v>28811.55211809349</v>
+        <v>28811.552</v>
       </c>
       <c r="L29">
-        <v>2127553.840071435</v>
+        <v>2127553.84</v>
       </c>
       <c r="M29">
-        <v>2067778.62225</v>
+        <v>2067778.622</v>
       </c>
       <c r="N29">
-        <v>1.028907938779438</v>
+        <v>1.029</v>
       </c>
     </row>
     <row r="30">
@@ -12954,40 +12954,40 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>104.2365139551491</v>
+        <v>104.237</v>
       </c>
       <c r="D30">
-        <v>7904807.432524236</v>
+        <v>7904807.433</v>
       </c>
       <c r="E30">
-        <v>18483.00911153623</v>
+        <v>18483.009</v>
       </c>
       <c r="F30">
-        <v>0.02218288807378074</v>
+        <v>0.022</v>
       </c>
       <c r="G30">
-        <v>604942.6973134157</v>
+        <v>604942.697</v>
       </c>
       <c r="H30">
         <v>2900751.439</v>
       </c>
       <c r="I30">
-        <v>0.01141877615877212</v>
+        <v>0.011</v>
       </c>
       <c r="J30">
-        <v>3069835.753369031</v>
+        <v>3069835.753</v>
       </c>
       <c r="K30">
-        <v>29450.67555396106</v>
+        <v>29450.676</v>
       </c>
       <c r="L30">
-        <v>2240980.099959393</v>
+        <v>2240980.1</v>
       </c>
       <c r="M30">
-        <v>2175563.57925</v>
+        <v>2175563.579</v>
       </c>
       <c r="N30">
-        <v>1.030068769919353</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="31">
@@ -12998,40 +12998,40 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>107.4109884085924</v>
+        <v>107.411</v>
       </c>
       <c r="D31">
-        <v>8356074.073565523</v>
+        <v>8356074.074</v>
       </c>
       <c r="E31">
-        <v>18856.390663316</v>
+        <v>18856.391</v>
       </c>
       <c r="F31">
-        <v>0.02206062237225026</v>
+        <v>0.022</v>
       </c>
       <c r="G31">
-        <v>642141.7044882596</v>
+        <v>642141.704</v>
       </c>
       <c r="H31">
         <v>3051807.985</v>
       </c>
       <c r="I31">
-        <v>0.01123943098566664</v>
+        <v>0.011</v>
       </c>
       <c r="J31">
-        <v>3233111.114640527</v>
+        <v>3233111.115</v>
       </c>
       <c r="K31">
-        <v>30100.37578596466</v>
+        <v>30100.376</v>
       </c>
       <c r="L31">
-        <v>2360171.113687584</v>
+        <v>2360171.114</v>
       </c>
       <c r="M31">
-        <v>2288855.98875</v>
+        <v>2288855.989</v>
       </c>
       <c r="N31">
-        <v>1.031157541273067</v>
+        <v>1.031</v>
       </c>
     </row>
     <row r="32">
@@ -13042,40 +13042,40 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>110.6821400020627</v>
+        <v>110.682</v>
       </c>
       <c r="D32">
-        <v>8830108.889283033</v>
+        <v>8830108.889</v>
       </c>
       <c r="E32">
-        <v>19237.31502278299</v>
+        <v>19237.315</v>
       </c>
       <c r="F32">
-        <v>0.02194630423182679</v>
+        <v>0.022</v>
       </c>
       <c r="G32">
-        <v>681118.2586015398</v>
+        <v>681118.259</v>
       </c>
       <c r="H32">
         <v>3210584.669</v>
       </c>
       <c r="I32">
-        <v>0.0110797662733119</v>
+        <v>0.011</v>
       </c>
       <c r="J32">
-        <v>3404689.743582165</v>
+        <v>3404689.744</v>
       </c>
       <c r="K32">
-        <v>30760.96779045575</v>
+        <v>30760.968</v>
       </c>
       <c r="L32">
-        <v>2485423.512814981</v>
+        <v>2485423.513</v>
       </c>
       <c r="M32">
-        <v>2407938.50175</v>
+        <v>2407938.502</v>
       </c>
       <c r="N32">
-        <v>1.032178982564823</v>
+        <v>1.032</v>
       </c>
     </row>
     <row r="33">
@@ -13086,40 +13086,40 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>114.0529129928035</v>
+        <v>114.053</v>
       </c>
       <c r="D33">
-        <v>9328076.969607253</v>
+        <v>9328076.970000001</v>
       </c>
       <c r="E33">
-        <v>19625.93456476005</v>
+        <v>19625.935</v>
       </c>
       <c r="F33">
-        <v>0.0218393692341054</v>
+        <v>0.022</v>
       </c>
       <c r="G33">
-        <v>721967.3231291215</v>
+        <v>721967.323</v>
       </c>
       <c r="H33">
         <v>3377477.67</v>
       </c>
       <c r="I33">
-        <v>0.01093793634787223</v>
+        <v>0.011</v>
       </c>
       <c r="J33">
-        <v>3584998.74516237</v>
+        <v>3584998.745</v>
       </c>
       <c r="K33">
-        <v>31432.76792402994</v>
+        <v>31432.768</v>
       </c>
       <c r="L33">
-        <v>2617049.08396853</v>
+        <v>2617049.084</v>
       </c>
       <c r="M33">
-        <v>2533108.2525</v>
+        <v>2533108.252</v>
       </c>
       <c r="N33">
-        <v>1.033137482926632</v>
+        <v>1.033</v>
       </c>
     </row>
     <row r="34">
@@ -13130,40 +13130,40 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>117.5263413040403</v>
+        <v>117.526</v>
       </c>
       <c r="D34">
-        <v>9851203.577113554</v>
+        <v>9851203.577</v>
       </c>
       <c r="E34">
-        <v>20022.40474224563</v>
+        <v>20022.405</v>
       </c>
       <c r="F34">
-        <v>0.0217392986883052</v>
+        <v>0.022</v>
       </c>
       <c r="G34">
-        <v>764788.6051072041</v>
+        <v>764788.605</v>
       </c>
       <c r="H34">
         <v>3552903.469</v>
       </c>
       <c r="I34">
-        <v>0.01081225010502005</v>
+        <v>0.011</v>
       </c>
       <c r="J34">
-        <v>3774487.054710691</v>
+        <v>3774487.055</v>
       </c>
       <c r="K34">
-        <v>32116.0942545306</v>
+        <v>32116.094</v>
       </c>
       <c r="L34">
-        <v>2755375.549938805</v>
+        <v>2755375.55</v>
       </c>
       <c r="M34">
-        <v>2664677.60175</v>
+        <v>2664677.602</v>
       </c>
       <c r="N34">
-        <v>1.034037118835404</v>
+        <v>1.034</v>
       </c>
     </row>
     <row r="35">
@@ -13174,40 +13174,40 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>121.1055512557168</v>
+        <v>121.106</v>
       </c>
       <c r="D35">
-        <v>10400777.19770668</v>
+        <v>10400777.198</v>
       </c>
       <c r="E35">
-        <v>20426.88414859706</v>
+        <v>20426.884</v>
       </c>
       <c r="F35">
-        <v>0.02164561527101908</v>
+        <v>0.022</v>
       </c>
       <c r="G35">
-        <v>809686.8019971297</v>
+        <v>809686.802</v>
       </c>
       <c r="H35">
         <v>3737299.886</v>
       </c>
       <c r="I35">
-        <v>0.01070115631748902</v>
+        <v>0.011</v>
       </c>
       <c r="J35">
-        <v>3973626.562267698</v>
+        <v>3973626.562</v>
       </c>
       <c r="K35">
-        <v>32811.26687477196</v>
+        <v>32811.267</v>
       </c>
       <c r="L35">
-        <v>2900747.390455419</v>
+        <v>2900747.39</v>
       </c>
       <c r="M35">
-        <v>2802974.9145</v>
+        <v>2802974.914</v>
       </c>
       <c r="N35">
-        <v>1.034881680692052</v>
+        <v>1.035</v>
       </c>
     </row>
     <row r="36">
@@ -13218,40 +13218,40 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>124.7937643783934</v>
+        <v>124.794</v>
       </c>
       <c r="D36">
-        <v>10978152.75036534</v>
+        <v>10978152.75</v>
       </c>
       <c r="E36">
-        <v>20839.53458097002</v>
+        <v>20839.535</v>
       </c>
       <c r="F36">
-        <v>0.02155787915623905</v>
+        <v>0.022</v>
       </c>
       <c r="G36">
-        <v>856771.8611625985</v>
+        <v>856771.861</v>
       </c>
       <c r="H36">
         <v>3931127.183</v>
       </c>
       <c r="I36">
-        <v>0.01060323097960688</v>
+        <v>0.011</v>
       </c>
       <c r="J36">
-        <v>4182913.29412995</v>
+        <v>4182913.294</v>
       </c>
       <c r="K36">
-        <v>33518.6082010214</v>
+        <v>33518.608</v>
       </c>
       <c r="L36">
-        <v>3053526.704714864</v>
+        <v>3053526.705</v>
       </c>
       <c r="M36">
-        <v>2948345.38725</v>
+        <v>2948345.387</v>
       </c>
       <c r="N36">
-        <v>1.035674693310938</v>
+        <v>1.036</v>
       </c>
     </row>
     <row r="37">
@@ -13262,40 +13262,40 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>128.5943003128424</v>
+        <v>128.594</v>
       </c>
       <c r="D37">
-        <v>11584754.96388322</v>
+        <v>11584754.964</v>
       </c>
       <c r="E37">
-        <v>21260.52110503953</v>
+        <v>21260.521</v>
       </c>
       <c r="F37">
-        <v>0.02147568457202328</v>
+        <v>0.021</v>
       </c>
       <c r="G37">
-        <v>906159.2525986936</v>
+        <v>906159.253</v>
       </c>
       <c r="H37">
         <v>4134869.205</v>
       </c>
       <c r="I37">
-        <v>0.01051716637239311</v>
+        <v>0.011</v>
       </c>
       <c r="J37">
-        <v>4402868.654568579</v>
+        <v>4402868.655</v>
       </c>
       <c r="K37">
-        <v>34238.44325803977</v>
+        <v>34238.443</v>
       </c>
       <c r="L37">
-        <v>3214094.117835063</v>
+        <v>3214094.118</v>
       </c>
       <c r="M37">
-        <v>3101151.90375</v>
+        <v>3101151.904</v>
       </c>
       <c r="N37">
-        <v>1.036419439482629</v>
+        <v>1.036</v>
       </c>
     </row>
     <row r="38">
@@ -13306,40 +13306,40 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>132.5105797979486</v>
+        <v>132.511</v>
       </c>
       <c r="D38">
-        <v>12222081.92897003</v>
+        <v>12222081.929</v>
       </c>
       <c r="E38">
-        <v>21690.01212102845</v>
+        <v>21690.012</v>
       </c>
       <c r="F38">
-        <v>0.02139865672947981</v>
+        <v>0.021</v>
       </c>
       <c r="G38">
-        <v>957970.2555861175</v>
+        <v>957970.2560000001</v>
       </c>
       <c r="H38">
         <v>4349034.601</v>
       </c>
       <c r="I38">
-        <v>0.01044176157565477</v>
+        <v>0.01</v>
       </c>
       <c r="J38">
-        <v>4634040.730847355</v>
+        <v>4634040.731</v>
       </c>
       <c r="K38">
-        <v>34971.09995227034</v>
+        <v>34971.1</v>
       </c>
       <c r="L38">
-        <v>3382849.733518569</v>
+        <v>3382849.734</v>
       </c>
       <c r="M38">
-        <v>3261775.95075</v>
+        <v>3261775.951</v>
       </c>
       <c r="N38">
-        <v>1.037118975857533</v>
+        <v>1.037</v>
       </c>
     </row>
     <row r="39">
@@ -13350,40 +13350,40 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>136.5461277496054</v>
+        <v>136.546</v>
       </c>
       <c r="D39">
-        <v>12891708.83452307</v>
+        <v>12891708.835</v>
       </c>
       <c r="E39">
-        <v>21898.57934010054</v>
+        <v>21898.579</v>
       </c>
       <c r="F39">
-        <v>0.01421411618151222</v>
+        <v>0.014</v>
       </c>
       <c r="G39">
-        <v>1012332.25997962</v>
+        <v>1012332.26</v>
       </c>
       <c r="H39">
         <v>4419630.739</v>
       </c>
       <c r="I39">
-        <v>0.01037591419052204</v>
+        <v>0.01</v>
       </c>
       <c r="J39">
-        <v>4843043.078368242</v>
+        <v>4843043.078</v>
       </c>
       <c r="K39">
-        <v>35468.18322998718</v>
+        <v>35468.183</v>
       </c>
       <c r="L39">
-        <v>3535421.447208817</v>
+        <v>3535421.447</v>
       </c>
       <c r="M39">
-        <v>3314723.05425</v>
+        <v>3314723.054</v>
       </c>
       <c r="N39">
-        <v>1.066581246561714</v>
+        <v>1.067</v>
       </c>
     </row>
     <row r="40">
@@ -13394,40 +13394,40 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>140.704576433377</v>
+        <v>140.705</v>
       </c>
       <c r="D40">
-        <v>13586801.2507342</v>
+        <v>13586801.251</v>
       </c>
       <c r="E40">
-        <v>22340.9599874528</v>
+        <v>22340.96</v>
       </c>
       <c r="F40">
-        <v>0.02104822109637444</v>
+        <v>0.021</v>
       </c>
       <c r="G40">
-        <v>1068699.8311478</v>
+        <v>1068699.831</v>
       </c>
       <c r="H40">
         <v>4643713.181</v>
       </c>
       <c r="I40">
-        <v>0.0103038123516806</v>
+        <v>0.01</v>
       </c>
       <c r="J40">
-        <v>5095577.597002588</v>
+        <v>5095577.597</v>
       </c>
       <c r="K40">
-        <v>36214.72539249867</v>
+        <v>36214.725</v>
       </c>
       <c r="L40">
-        <v>3719771.645811889</v>
+        <v>3719771.646</v>
       </c>
       <c r="M40">
-        <v>3482784.88575</v>
+        <v>3482784.886</v>
       </c>
       <c r="N40">
-        <v>1.068045190224505</v>
+        <v>1.068</v>
       </c>
     </row>
     <row r="41">
@@ -13438,40 +13438,40 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>144.9896687337825</v>
+        <v>144.99</v>
       </c>
       <c r="D41">
-        <v>14317223.59995548</v>
+        <v>14317223.6</v>
       </c>
       <c r="E41">
-        <v>22792.27731668348</v>
+        <v>22792.277</v>
       </c>
       <c r="F41">
-        <v>0.02099767651919819</v>
+        <v>0.021</v>
       </c>
       <c r="G41">
-        <v>1127863.38984194</v>
+        <v>1127863.39</v>
       </c>
       <c r="H41">
         <v>4879308.171</v>
       </c>
       <c r="I41">
-        <v>0.01025678114428015</v>
+        <v>0.01</v>
       </c>
       <c r="J41">
-        <v>5361014.819697626</v>
+        <v>5361014.82</v>
       </c>
       <c r="K41">
-        <v>36975.15048152195</v>
+        <v>36975.15</v>
       </c>
       <c r="L41">
-        <v>3913540.818379267</v>
+        <v>3913540.818</v>
       </c>
       <c r="M41">
-        <v>3659481.12825</v>
+        <v>3659481.128</v>
       </c>
       <c r="N41">
-        <v>1.06942505815046</v>
+        <v>1.069</v>
       </c>
     </row>
     <row r="42">
@@ -13482,40 +13482,40 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>149.4052615231446</v>
+        <v>149.405</v>
       </c>
       <c r="D42">
-        <v>15084788.36088167</v>
+        <v>15084788.361</v>
       </c>
       <c r="E42">
-        <v>23252.71186074192</v>
+        <v>23252.712</v>
       </c>
       <c r="F42">
-        <v>0.02095022042392075</v>
+        <v>0.021</v>
       </c>
       <c r="G42">
-        <v>1189969.150642215</v>
+        <v>1189969.151</v>
       </c>
       <c r="H42">
         <v>5127005.823</v>
       </c>
       <c r="I42">
-        <v>0.01021609181530004</v>
+        <v>0.01</v>
       </c>
       <c r="J42">
-        <v>5640016.953710478</v>
+        <v>5640016.954</v>
       </c>
       <c r="K42">
-        <v>37749.78803431748</v>
+        <v>37749.788</v>
       </c>
       <c r="L42">
-        <v>4117212.376208649</v>
+        <v>4117212.376</v>
       </c>
       <c r="M42">
-        <v>3845254.36725</v>
+        <v>3845254.367</v>
       </c>
       <c r="N42">
-        <v>1.070725622542663</v>
+        <v>1.071</v>
       </c>
     </row>
     <row r="43">
@@ -13526,40 +13526,40 @@
         <v>1</v>
       </c>
       <c r="C43">
-        <v>153.9553291330353</v>
+        <v>153.955</v>
       </c>
       <c r="D43">
-        <v>15891401.06487402</v>
+        <v>15891401.065</v>
       </c>
       <c r="E43">
-        <v>23480.9287703151</v>
+        <v>23480.929</v>
       </c>
       <c r="F43">
-        <v>0.01393000839746998</v>
+        <v>0.014</v>
       </c>
       <c r="G43">
-        <v>1255170.723690736</v>
+        <v>1255170.724</v>
       </c>
       <c r="H43">
         <v>5205424.762</v>
       </c>
       <c r="I43">
-        <v>0.01018103322685211</v>
+        <v>0.01</v>
       </c>
       <c r="J43">
-        <v>5892739.200238374</v>
+        <v>5892739.2</v>
       </c>
       <c r="K43">
-        <v>38275.64289863823</v>
+        <v>38275.643</v>
       </c>
       <c r="L43">
-        <v>4301699.616174013</v>
+        <v>4301699.616</v>
       </c>
       <c r="M43">
-        <v>3904068.5715</v>
+        <v>3904068.572</v>
       </c>
       <c r="N43">
-        <v>1.10185042536823</v>
+        <v>1.102</v>
       </c>
     </row>
     <row r="44">
@@ -13570,40 +13570,40 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>158.6439669314422</v>
+        <v>158.644</v>
       </c>
       <c r="D44">
-        <v>16728929.82233866</v>
+        <v>16728929.822</v>
       </c>
       <c r="E44">
-        <v>23955.27499654827</v>
+        <v>23955.275</v>
       </c>
       <c r="F44">
-        <v>0.02065977933472664</v>
+        <v>0.021</v>
       </c>
       <c r="G44">
-        <v>1322818.678747874</v>
+        <v>1322818.679</v>
       </c>
       <c r="H44">
         <v>5464743.929</v>
       </c>
       <c r="I44">
-        <v>0.01014302896864769</v>
+        <v>0.01</v>
       </c>
       <c r="J44">
-        <v>6197650.134778797</v>
+        <v>6197650.135</v>
       </c>
       <c r="K44">
-        <v>39066.40923481889</v>
+        <v>39066.409</v>
       </c>
       <c r="L44">
-        <v>4524284.598388522</v>
+        <v>4524284.598</v>
       </c>
       <c r="M44">
-        <v>4098557.94675</v>
+        <v>4098557.947</v>
       </c>
       <c r="N44">
-        <v>1.103872302690293</v>
+        <v>1.104</v>
       </c>
     </row>
     <row r="45">
@@ -13614,40 +13614,40 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>163.4753950088764</v>
+        <v>163.475</v>
       </c>
       <c r="D45">
-        <v>17609185.16313981</v>
+        <v>17609185.163</v>
       </c>
       <c r="E45">
-        <v>24439.20365218798</v>
+        <v>24439.204</v>
       </c>
       <c r="F45">
-        <v>0.02063273620809719</v>
+        <v>0.021</v>
       </c>
       <c r="G45">
-        <v>1393858.934293535</v>
+        <v>1393858.934</v>
       </c>
       <c r="H45">
         <v>5737423.67</v>
       </c>
       <c r="I45">
-        <v>0.01011887184620173</v>
+        <v>0.01</v>
       </c>
       <c r="J45">
-        <v>6518165.519284738</v>
+        <v>6518165.519</v>
       </c>
       <c r="K45">
-        <v>39872.45615115848</v>
+        <v>39872.456</v>
       </c>
       <c r="L45">
-        <v>4758260.829077859</v>
+        <v>4758260.829</v>
       </c>
       <c r="M45">
-        <v>4303067.7525</v>
+        <v>4303067.752</v>
       </c>
       <c r="N45">
-        <v>1.105783385891008</v>
+        <v>1.106</v>
       </c>
     </row>
     <row r="46">
@@ -13658,40 +13658,40 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>168.4539619767388</v>
+        <v>168.454</v>
       </c>
       <c r="D46">
-        <v>18534359.1364354</v>
+        <v>18534359.136</v>
       </c>
       <c r="E46">
-        <v>24932.90831514896</v>
+        <v>24932.908</v>
       </c>
       <c r="F46">
-        <v>0.02060730919695159</v>
+        <v>0.021</v>
       </c>
       <c r="G46">
-        <v>1468467.887307488</v>
+        <v>1468467.887</v>
       </c>
       <c r="H46">
         <v>6024148.98</v>
       </c>
       <c r="I46">
-        <v>0.01009829546294735</v>
+        <v>0.01</v>
       </c>
       <c r="J46">
-        <v>6855085.774069377</v>
+        <v>6855085.774</v>
       </c>
       <c r="K46">
-        <v>40694.1201835073</v>
+        <v>40694.12</v>
       </c>
       <c r="L46">
-        <v>5004212.615070646</v>
+        <v>5004212.615</v>
       </c>
       <c r="M46">
         <v>4518111.735</v>
       </c>
       <c r="N46">
-        <v>1.107589388793778</v>
+        <v>1.108</v>
       </c>
     </row>
     <row r="47">
@@ -13702,40 +13702,40 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>173.5841488813638</v>
+        <v>173.584</v>
       </c>
       <c r="D47">
-        <v>19506756.21449533</v>
+        <v>19506756.214</v>
       </c>
       <c r="E47">
-        <v>25436.58647387921</v>
+        <v>25436.586</v>
       </c>
       <c r="F47">
-        <v>0.02058339933861238</v>
+        <v>0.021</v>
       </c>
       <c r="G47">
-        <v>1546830.887296576</v>
+        <v>1546830.887</v>
       </c>
       <c r="H47">
         <v>6325639.936</v>
       </c>
       <c r="I47">
-        <v>0.010080855352283</v>
+        <v>0.01</v>
       </c>
       <c r="J47">
-        <v>7209252.348738623</v>
+        <v>7209252.349</v>
       </c>
       <c r="K47">
-        <v>41531.74350997792</v>
+        <v>41531.744</v>
       </c>
       <c r="L47">
-        <v>5262754.214579195</v>
+        <v>5262754.215</v>
       </c>
       <c r="M47">
         <v>4744229.952</v>
       </c>
       <c r="N47">
-        <v>1.10929576935043</v>
+        <v>1.109</v>
       </c>
     </row>
     <row r="48">
@@ -13746,40 +13746,40 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>178.8705732372636</v>
+        <v>178.871</v>
       </c>
       <c r="D48">
-        <v>20528799.05310017</v>
+        <v>20528799.053</v>
       </c>
       <c r="E48">
-        <v>25950.43960635802</v>
+        <v>25950.44</v>
       </c>
       <c r="F48">
-        <v>0.02056091400219765</v>
+        <v>0.021</v>
       </c>
       <c r="G48">
-        <v>1629142.698779486</v>
+        <v>1629142.699</v>
       </c>
       <c r="H48">
         <v>6642653.499</v>
       </c>
       <c r="I48">
-        <v>0.01006614918308803</v>
+        <v>0.01</v>
       </c>
       <c r="J48">
-        <v>7581549.826292658</v>
+        <v>7581549.826</v>
       </c>
       <c r="K48">
-        <v>42385.6741166479</v>
+        <v>42385.674</v>
       </c>
       <c r="L48">
-        <v>5534531.37319364</v>
+        <v>5534531.373</v>
       </c>
       <c r="M48">
-        <v>4981990.12425</v>
+        <v>4981990.124</v>
       </c>
       <c r="N48">
-        <v>1.110907736700265</v>
+        <v>1.111</v>
       </c>
     </row>
     <row r="49">
@@ -13790,40 +13790,40 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>184.3179931832029</v>
+        <v>184.318</v>
       </c>
       <c r="D49">
-        <v>21603034.54754933</v>
+        <v>21603034.548</v>
       </c>
       <c r="E49">
-        <v>26474.67326068985</v>
+        <v>26474.673</v>
       </c>
       <c r="F49">
-        <v>0.02053976645271118</v>
+        <v>0.021</v>
       </c>
       <c r="G49">
-        <v>1715607.987354159</v>
+        <v>1715607.987</v>
       </c>
       <c r="H49">
         <v>6975985.407</v>
       </c>
       <c r="I49">
-        <v>0.01005381437428294</v>
+        <v>0.01</v>
       </c>
       <c r="J49">
-        <v>7972908.135073148</v>
+        <v>7972908.135</v>
       </c>
       <c r="K49">
-        <v>43256.26596394458</v>
+        <v>43256.266</v>
       </c>
       <c r="L49">
-        <v>5820222.938603398</v>
+        <v>5820222.939</v>
       </c>
       <c r="M49">
-        <v>5231989.05525</v>
+        <v>5231989.055</v>
       </c>
       <c r="N49">
-        <v>1.112430258768057</v>
+        <v>1.112</v>
       </c>
     </row>
     <row r="50">
@@ -13834,40 +13834,40 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>189.9313117648449</v>
+        <v>189.931</v>
       </c>
       <c r="D50">
-        <v>22732140.19941564</v>
+        <v>22732140.199</v>
       </c>
       <c r="E50">
-        <v>27009.4971373263</v>
+        <v>27009.497</v>
       </c>
       <c r="F50">
-        <v>0.02051987544857537</v>
+        <v>0.021</v>
       </c>
       <c r="G50">
-        <v>1806441.830561456</v>
+        <v>1806441.831</v>
       </c>
       <c r="H50">
         <v>7326472.166</v>
       </c>
       <c r="I50">
-        <v>0.01004352571528752</v>
+        <v>0.01</v>
       </c>
       <c r="J50">
-        <v>8384304.874088099</v>
+        <v>8384304.874</v>
       </c>
       <c r="K50">
-        <v>44143.87915389517</v>
+        <v>44143.879</v>
       </c>
       <c r="L50">
-        <v>6120542.558084312</v>
+        <v>6120542.558</v>
       </c>
       <c r="M50">
-        <v>5494854.1245</v>
+        <v>5494854.124</v>
       </c>
       <c r="N50">
-        <v>1.11386806990827</v>
+        <v>1.114</v>
       </c>
     </row>
     <row r="51">
@@ -13878,40 +13878,40 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>195.7155813478234</v>
+        <v>195.716</v>
       </c>
       <c r="D51">
-        <v>23918930.80996104</v>
+        <v>23918930.81</v>
       </c>
       <c r="E51">
-        <v>27555.12517294912</v>
+        <v>27555.125</v>
       </c>
       <c r="F51">
-        <v>0.0205011648696579</v>
+        <v>0.021</v>
       </c>
       <c r="G51">
-        <v>1901870.25482076</v>
+        <v>1901870.255</v>
       </c>
       <c r="H51">
         <v>7694993.141</v>
       </c>
       <c r="I51">
-        <v>0.01003499298595262</v>
+        <v>0.01</v>
       </c>
       <c r="J51">
-        <v>8816767.757529765</v>
+        <v>8816767.757999999</v>
       </c>
       <c r="K51">
-        <v>45048.88009841543</v>
+        <v>45048.88</v>
       </c>
       <c r="L51">
-        <v>6436240.462996729</v>
+        <v>6436240.463</v>
       </c>
       <c r="M51">
-        <v>5771244.85575</v>
+        <v>5771244.856</v>
       </c>
       <c r="N51">
-        <v>1.115225679011727</v>
+        <v>1.115</v>
       </c>
     </row>
     <row r="52">
@@ -13922,40 +13922,40 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>201.6760081652129</v>
+        <v>201.676</v>
       </c>
       <c r="D52">
-        <v>25166365.51694503</v>
+        <v>25166365.517</v>
       </c>
       <c r="E52">
-        <v>28111.77562604768</v>
+        <v>28111.776</v>
       </c>
       <c r="F52">
-        <v>0.02048356337316214</v>
+        <v>0.02</v>
       </c>
       <c r="G52">
-        <v>2002130.799778525</v>
+        <v>2002130.8</v>
       </c>
       <c r="H52">
         <v>8082472.756</v>
       </c>
       <c r="I52">
-        <v>0.01002795857615139</v>
+        <v>0.01</v>
       </c>
       <c r="J52">
-        <v>9271377.184598934</v>
+        <v>9271377.185000001</v>
       </c>
       <c r="K52">
-        <v>45971.64168880131</v>
+        <v>45971.642</v>
       </c>
       <c r="L52">
-        <v>6768105.344757222</v>
+        <v>6768105.345</v>
       </c>
       <c r="M52">
         <v>6061854.567</v>
       </c>
       <c r="N52">
-        <v>1.116507377396014</v>
+        <v>1.117</v>
       </c>
     </row>
     <row r="53">
@@ -13966,40 +13966,40 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>207.8179570034902</v>
+        <v>207.818</v>
       </c>
       <c r="D53">
-        <v>26477555.19241697</v>
+        <v>26477555.192</v>
       </c>
       <c r="E53">
-        <v>28392.23790410678</v>
+        <v>28392.238</v>
       </c>
       <c r="F53">
-        <v>0.0136033180250314</v>
+        <v>0.014</v>
       </c>
       <c r="G53">
-        <v>2107473.111479362</v>
+        <v>2107473.111</v>
       </c>
       <c r="H53">
         <v>8203071.763</v>
       </c>
       <c r="I53">
-        <v>0.01002219511069917</v>
+        <v>0.01</v>
       </c>
       <c r="J53">
-        <v>9683695.119507</v>
+        <v>9683695.119999999</v>
       </c>
       <c r="K53">
-        <v>46597.00855082686</v>
+        <v>46597.009</v>
       </c>
       <c r="L53">
-        <v>7069097.43724011</v>
+        <v>7069097.437</v>
       </c>
       <c r="M53">
-        <v>6152303.82225</v>
+        <v>6152303.822</v>
       </c>
       <c r="N53">
-        <v>1.149016310227479</v>
+        <v>1.149</v>
       </c>
     </row>
     <row r="54">
@@ -14010,40 +14010,40 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>214.1469560312034</v>
+        <v>214.147</v>
       </c>
       <c r="D54">
-        <v>27839376.76459704</v>
+        <v>27839376.765</v>
       </c>
       <c r="E54">
-        <v>28675.67018562514</v>
+        <v>28675.67</v>
       </c>
       <c r="F54">
-        <v>0.01339502701117423</v>
+        <v>0.013</v>
       </c>
       <c r="G54">
-        <v>2216848.089410328</v>
+        <v>2216848.089</v>
       </c>
       <c r="H54">
         <v>8317991.973</v>
       </c>
       <c r="I54">
-        <v>0.01001625982902188</v>
+        <v>0.01</v>
       </c>
       <c r="J54">
-        <v>10112271.25886941</v>
+        <v>10112271.259</v>
       </c>
       <c r="K54">
-        <v>47221.1767390051</v>
+        <v>47221.177</v>
       </c>
       <c r="L54">
-        <v>7381958.018974671</v>
+        <v>7381958.019</v>
       </c>
       <c r="M54">
-        <v>6238493.97975</v>
+        <v>6238493.98</v>
       </c>
       <c r="N54">
-        <v>1.183291679520142</v>
+        <v>1.183</v>
       </c>
     </row>
     <row r="55">
@@ -14054,40 +14054,40 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>220.668701774698</v>
+        <v>220.669</v>
       </c>
       <c r="D55">
-        <v>29253869.50873051</v>
+        <v>29253869.509</v>
       </c>
       <c r="E55">
-        <v>29254.95714954006</v>
+        <v>29254.957</v>
       </c>
       <c r="F55">
-        <v>0.02005335452877582</v>
+        <v>0.02</v>
       </c>
       <c r="G55">
-        <v>2330419.591011303</v>
+        <v>2330419.591</v>
       </c>
       <c r="H55">
         <v>8722234.666999999</v>
       </c>
       <c r="I55">
-        <v>0.0100118202777181</v>
+        <v>0.01</v>
       </c>
       <c r="J55">
-        <v>10629196.44938431</v>
+        <v>10629196.449</v>
       </c>
       <c r="K55">
-        <v>48168.11973741835</v>
+        <v>48168.12</v>
       </c>
       <c r="L55">
-        <v>7759313.408050548</v>
+        <v>7759313.408</v>
       </c>
       <c r="M55">
-        <v>6541676.00025</v>
+        <v>6541676</v>
       </c>
       <c r="N55">
-        <v>1.186135389119549</v>
+        <v>1.186</v>
       </c>
     </row>
     <row r="56">
@@ -14098,40 +14098,40 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>227.389064245374</v>
+        <v>227.389</v>
       </c>
       <c r="D56">
-        <v>30741013.84072736</v>
+        <v>30741013.841</v>
       </c>
       <c r="E56">
-        <v>29845.94648638609</v>
+        <v>29845.946</v>
       </c>
       <c r="F56">
-        <v>0.02006192348873608</v>
+        <v>0.02</v>
       </c>
       <c r="G56">
-        <v>2449786.736358537</v>
+        <v>2449786.736</v>
       </c>
       <c r="H56">
         <v>9147369.954</v>
       </c>
       <c r="I56">
-        <v>0.01000923235936716</v>
+        <v>0.01</v>
       </c>
       <c r="J56">
-        <v>11172639.98902896</v>
+        <v>11172639.989</v>
       </c>
       <c r="K56">
-        <v>49134.46487018672</v>
+        <v>49134.465</v>
       </c>
       <c r="L56">
-        <v>8156027.191991141</v>
+        <v>8156027.192</v>
       </c>
       <c r="M56">
-        <v>6860527.4655</v>
+        <v>6860527.466</v>
       </c>
       <c r="N56">
-        <v>1.188833837194867</v>
+        <v>1.189</v>
       </c>
     </row>
     <row r="57">
@@ -14142,40 +14142,40 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>234.3140922230932</v>
+        <v>234.314</v>
       </c>
       <c r="D57">
-        <v>32304533.28435551</v>
+        <v>32304533.284</v>
       </c>
       <c r="E57">
-        <v>30448.87459977793</v>
+        <v>30448.875</v>
       </c>
       <c r="F57">
-        <v>0.0200699984126651</v>
+        <v>0.02</v>
       </c>
       <c r="G57">
-        <v>2575248.066684775</v>
+        <v>2575248.067</v>
       </c>
       <c r="H57">
         <v>9594470.606000001</v>
       </c>
       <c r="I57">
-        <v>0.01000715753977381</v>
+        <v>0.01</v>
       </c>
       <c r="J57">
-        <v>11743961.36813625</v>
+        <v>11743961.368</v>
       </c>
       <c r="K57">
-        <v>50120.59350213852</v>
+        <v>50120.594</v>
       </c>
       <c r="L57">
-        <v>8573091.798739461</v>
+        <v>8573091.799000001</v>
       </c>
       <c r="M57">
-        <v>7195852.954500001</v>
+        <v>7195852.955</v>
       </c>
       <c r="N57">
-        <v>1.191393411308966</v>
+        <v>1.191</v>
       </c>
     </row>
     <row r="58">
@@ -14186,40 +14186,40 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>241.4500187004888</v>
+        <v>241.45</v>
       </c>
       <c r="D58">
-        <v>33948342.29501535</v>
+        <v>33948342.295</v>
       </c>
       <c r="E58">
-        <v>31063.98266900009</v>
+        <v>31063.983</v>
       </c>
       <c r="F58">
-        <v>0.02007760754279531</v>
+        <v>0.02</v>
       </c>
       <c r="G58">
-        <v>2707117.371380108</v>
+        <v>2707117.371</v>
       </c>
       <c r="H58">
         <v>10064664.203</v>
       </c>
       <c r="I58">
-        <v>0.01000550654346758</v>
+        <v>0.01</v>
       </c>
       <c r="J58">
-        <v>12344589.77999369</v>
+        <v>12344589.78</v>
       </c>
       <c r="K58">
-        <v>51126.89510828643</v>
+        <v>51126.895</v>
       </c>
       <c r="L58">
-        <v>9011550.539395394</v>
+        <v>9011550.539000001</v>
       </c>
       <c r="M58">
-        <v>7548498.152249999</v>
+        <v>7548498.152</v>
       </c>
       <c r="N58">
-        <v>1.193820327916395</v>
+        <v>1.194</v>
       </c>
     </row>
     <row r="59">
@@ -14230,40 +14230,40 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>248.8032664930802</v>
+        <v>248.803</v>
       </c>
       <c r="D59">
-        <v>35676556.04821315</v>
+        <v>35676556.048</v>
       </c>
       <c r="E59">
-        <v>31691.51674548181</v>
+        <v>31691.517</v>
       </c>
       <c r="F59">
-        <v>0.02008477753398972</v>
+        <v>0.02</v>
       </c>
       <c r="G59">
-        <v>2845724.472124778</v>
+        <v>2845724.472</v>
       </c>
       <c r="H59">
         <v>10559135.951</v>
       </c>
       <c r="I59">
-        <v>0.01000420294710096</v>
+        <v>0.01</v>
       </c>
       <c r="J59">
-        <v>12976027.69464834</v>
+        <v>12976027.695</v>
       </c>
       <c r="K59">
-        <v>52153.76742253999</v>
+        <v>52153.767</v>
       </c>
       <c r="L59">
-        <v>9472500.217093289</v>
+        <v>9472500.217</v>
       </c>
       <c r="M59">
-        <v>7919351.96325</v>
+        <v>7919351.963</v>
       </c>
       <c r="N59">
-        <v>1.196120624648421</v>
+        <v>1.196</v>
       </c>
     </row>
     <row r="60">
@@ -14274,40 +14274,40 @@
         <v>1</v>
       </c>
       <c r="C60">
-        <v>256.3804540202396</v>
+        <v>256.38</v>
       </c>
       <c r="D60">
-        <v>37493500.72994672</v>
+        <v>37493500.73</v>
       </c>
       <c r="E60">
-        <v>32008.30769776987</v>
+        <v>32008.308</v>
       </c>
       <c r="F60">
-        <v>0.0132434109629181</v>
+        <v>0.013</v>
       </c>
       <c r="G60">
-        <v>2991416.047132753</v>
+        <v>2991416.047</v>
       </c>
       <c r="H60">
         <v>10704848.822</v>
       </c>
       <c r="I60">
-        <v>0.01000318185713126</v>
+        <v>0.01</v>
       </c>
       <c r="J60">
-        <v>13548286.95434206</v>
+        <v>13548286.954</v>
       </c>
       <c r="K60">
-        <v>52844.46119778114</v>
+        <v>52844.461</v>
       </c>
       <c r="L60">
-        <v>9890249.476669705</v>
+        <v>9890249.477</v>
       </c>
       <c r="M60">
-        <v>8028636.616500001</v>
+        <v>8028636.617</v>
       </c>
       <c r="N60">
-        <v>1.231871605241645</v>
+        <v>1.232</v>
       </c>
     </row>
     <row r="61">
@@ -14318,40 +14318,40 @@
         <v>1</v>
       </c>
       <c r="C61">
-        <v>264.188401262217</v>
+        <v>264.188</v>
       </c>
       <c r="D61">
-        <v>39380832.43933436</v>
+        <v>39380832.439</v>
       </c>
       <c r="E61">
-        <v>32328.29811580917</v>
+        <v>32328.298</v>
       </c>
       <c r="F61">
-        <v>0.01305612838835502</v>
+        <v>0.013</v>
       </c>
       <c r="G61">
-        <v>3142725.144334285</v>
+        <v>3142725.144</v>
       </c>
       <c r="H61">
         <v>10843814.394</v>
       </c>
       <c r="I61">
-        <v>0.01000217747877837</v>
+        <v>0.01</v>
       </c>
       <c r="J61">
-        <v>14143168.94022179</v>
+        <v>14143168.94</v>
       </c>
       <c r="K61">
-        <v>53534.40526779281</v>
+        <v>53534.405</v>
       </c>
       <c r="L61">
-        <v>10324513.32636191</v>
+        <v>10324513.326</v>
       </c>
       <c r="M61">
-        <v>8132860.795499999</v>
+        <v>8132860.795</v>
       </c>
       <c r="N61">
-        <v>1.269481131667048</v>
+        <v>1.269</v>
       </c>
     </row>
     <row r="62">
@@ -14362,40 +14362,40 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>272.2341358985825</v>
+        <v>272.234</v>
       </c>
       <c r="D62">
-        <v>41341391.37681644</v>
+        <v>41341391.377</v>
       </c>
       <c r="E62">
-        <v>32981.37305853296</v>
+        <v>32981.373</v>
       </c>
       <c r="F62">
-        <v>0.01972506787444999</v>
+        <v>0.02</v>
       </c>
       <c r="G62">
-        <v>3299879.517365349</v>
+        <v>3299879.517</v>
       </c>
       <c r="H62">
         <v>11360200.068</v>
       </c>
       <c r="I62">
-        <v>0.01000147584721886</v>
+        <v>0.01</v>
       </c>
       <c r="J62">
-        <v>14861363.57884178</v>
+        <v>14861363.579</v>
       </c>
       <c r="K62">
-        <v>54590.37504531834</v>
+        <v>54590.375</v>
       </c>
       <c r="L62">
-        <v>10848795.4125545</v>
+        <v>10848795.413</v>
       </c>
       <c r="M62">
-        <v>8520150.050999999</v>
+        <v>8520150.051000001</v>
       </c>
       <c r="N62">
-        <v>1.273310369842746</v>
+        <v>1.273</v>
       </c>
     </row>
     <row r="63">
@@ -14406,40 +14406,40 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>280.5248996336122</v>
+        <v>280.525</v>
       </c>
       <c r="D63">
-        <v>43403076.61645422</v>
+        <v>43403076.616</v>
       </c>
       <c r="E63">
-        <v>33647.64099023767</v>
+        <v>33647.641</v>
       </c>
       <c r="F63">
-        <v>0.01975236546531713</v>
+        <v>0.02</v>
       </c>
       <c r="G63">
-        <v>3465111.608247571</v>
+        <v>3465111.608</v>
       </c>
       <c r="H63">
         <v>11903323.224</v>
       </c>
       <c r="I63">
-        <v>0.01000109457508082</v>
+        <v>0.01</v>
       </c>
       <c r="J63">
-        <v>15616446.40493004</v>
+        <v>15616446.405</v>
       </c>
       <c r="K63">
-        <v>55668.66408410219</v>
+        <v>55668.664</v>
       </c>
       <c r="L63">
-        <v>11400005.87559893</v>
+        <v>11400005.876</v>
       </c>
       <c r="M63">
         <v>8927492.418</v>
       </c>
       <c r="N63">
-        <v>1.27695497703406</v>
+        <v>1.277</v>
       </c>
     </row>
     <row r="64">
@@ -14450,40 +14450,40 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>289.068154714311</v>
+        <v>289.068</v>
       </c>
       <c r="D64">
-        <v>45571065.15302856</v>
+        <v>45571065.153</v>
       </c>
       <c r="E64">
-        <v>34327.36842697967</v>
+        <v>34327.368</v>
       </c>
       <c r="F64">
-        <v>0.01977812049452934</v>
+        <v>0.02</v>
       </c>
       <c r="G64">
-        <v>3638836.072016269</v>
+        <v>3638836.072</v>
       </c>
       <c r="H64">
         <v>12474559.706</v>
       </c>
       <c r="I64">
-        <v>0.01000080420526009</v>
+        <v>0.01</v>
       </c>
       <c r="J64">
-        <v>16410308.26881236</v>
+        <v>16410308.269</v>
       </c>
       <c r="K64">
-        <v>56769.68563012705</v>
+        <v>56769.686</v>
       </c>
       <c r="L64">
-        <v>11979525.03623303</v>
+        <v>11979525.036</v>
       </c>
       <c r="M64">
-        <v>9355919.7795</v>
+        <v>9355919.779999999</v>
       </c>
       <c r="N64">
-        <v>1.280421948730437</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="65">
@@ -14494,40 +14494,40 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>297.8715906469384</v>
+        <v>297.872</v>
       </c>
       <c r="D65">
-        <v>47850799.61411051</v>
+        <v>47850799.614</v>
       </c>
       <c r="E65">
-        <v>35020.8272687968</v>
+        <v>35020.827</v>
       </c>
       <c r="F65">
-        <v>0.01980241767532553</v>
+        <v>0.02</v>
       </c>
       <c r="G65">
-        <v>3821488.794511865</v>
+        <v>3821488.795</v>
       </c>
       <c r="H65">
         <v>13075355.466</v>
       </c>
       <c r="I65">
-        <v>0.01000058517211728</v>
+        <v>0.01</v>
       </c>
       <c r="J65">
-        <v>17244936.95811905</v>
+        <v>17244936.958</v>
       </c>
       <c r="K65">
-        <v>57893.86265627175</v>
+        <v>57893.863</v>
       </c>
       <c r="L65">
-        <v>12588803.97942691</v>
+        <v>12588803.979</v>
       </c>
       <c r="M65">
-        <v>9806516.599500001</v>
+        <v>9806516.6</v>
       </c>
       <c r="N65">
-        <v>1.283718214484924</v>
+        <v>1.284</v>
       </c>
     </row>
     <row r="66">
@@ -14538,40 +14538,40 @@
         <v>1</v>
       </c>
       <c r="C66">
-        <v>306.9431311180837</v>
+        <v>306.943</v>
       </c>
       <c r="D66">
-        <v>50248001.86907585</v>
+        <v>50248001.869</v>
       </c>
       <c r="E66">
-        <v>35370.99689739419</v>
+        <v>35370.997</v>
       </c>
       <c r="F66">
-        <v>0.01298089412985375</v>
+        <v>0.013</v>
       </c>
       <c r="G66">
-        <v>4013527.981893771</v>
+        <v>4013527.982</v>
       </c>
       <c r="H66">
         <v>13244163.12</v>
       </c>
       <c r="I66">
-        <v>0.01000042157044359</v>
+        <v>0.01</v>
       </c>
       <c r="J66">
-        <v>18000795.5677558</v>
+        <v>18000795.568</v>
       </c>
       <c r="K66">
-        <v>58645.3767581811</v>
+        <v>58645.377</v>
       </c>
       <c r="L66">
-        <v>13140580.76446174</v>
+        <v>13140580.764</v>
       </c>
       <c r="M66">
         <v>9933122.34</v>
       </c>
       <c r="N66">
-        <v>1.32290535792009</v>
+        <v>1.323</v>
       </c>
     </row>
     <row r="67">
@@ -14582,40 +14582,40 @@
         <v>0</v>
       </c>
       <c r="C67">
-        <v>316.2909411265182</v>
+        <v>316.291</v>
       </c>
       <c r="D67">
-        <v>52738280.68625176</v>
+        <v>52738280.686</v>
       </c>
       <c r="E67">
-        <v>36085.53843280378</v>
+        <v>36085.538</v>
       </c>
       <c r="F67">
-        <v>0.01965298988600888</v>
+        <v>0.02</v>
       </c>
       <c r="G67">
-        <v>4213002.773973137</v>
+        <v>4213002.774</v>
       </c>
       <c r="H67">
         <v>13873954.912</v>
       </c>
       <c r="I67">
-        <v>0.01000026867263672</v>
+        <v>0.01</v>
       </c>
       <c r="J67">
-        <v>18913544.74462276</v>
+        <v>18913544.745</v>
       </c>
       <c r="K67">
-        <v>59797.93375447082</v>
+        <v>59797.934</v>
       </c>
       <c r="L67">
-        <v>13806887.66357462</v>
+        <v>13806887.664</v>
       </c>
       <c r="M67">
         <v>10405466.184</v>
       </c>
       <c r="N67">
-        <v>1.326887947106572</v>
+        <v>1.327</v>
       </c>
     </row>
     <row r="68">
@@ -14626,40 +14626,40 @@
         <v>0</v>
       </c>
       <c r="C68">
-        <v>325.9234343322456</v>
+        <v>325.923</v>
       </c>
       <c r="D68">
-        <v>55357135.64495738</v>
+        <v>55357135.645</v>
       </c>
       <c r="E68">
-        <v>36814.51466473341</v>
+        <v>36814.515</v>
       </c>
       <c r="F68">
-        <v>0.01968434766140737</v>
+        <v>0.02</v>
       </c>
       <c r="G68">
-        <v>4422753.557906667</v>
+        <v>4422753.558</v>
       </c>
       <c r="H68">
         <v>14536359.521</v>
       </c>
       <c r="I68">
-        <v>0.01000019020173474</v>
+        <v>0.01</v>
       </c>
       <c r="J68">
-        <v>19873186.97254996</v>
+        <v>19873186.973</v>
       </c>
       <c r="K68">
-        <v>60975.01707192763</v>
+        <v>60975.017</v>
       </c>
       <c r="L68">
-        <v>14507426.48996147</v>
+        <v>14507426.49</v>
       </c>
       <c r="M68">
-        <v>10902269.64075</v>
+        <v>10902269.641</v>
       </c>
       <c r="N68">
-        <v>1.330679479411909</v>
+        <v>1.331</v>
       </c>
     </row>
     <row r="69">
@@ -14670,40 +14670,40 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>335.8492806293637</v>
+        <v>335.849</v>
       </c>
       <c r="D69">
-        <v>58111146.96229657</v>
+        <v>58111146.962</v>
       </c>
       <c r="E69">
-        <v>37182.63001955522</v>
+        <v>37182.63</v>
       </c>
       <c r="F69">
-        <v>0.01287044343087139</v>
+        <v>0.013</v>
       </c>
       <c r="G69">
-        <v>4643307.155041399</v>
+        <v>4643307.155</v>
       </c>
       <c r="H69">
         <v>14718441.895</v>
       </c>
       <c r="I69">
-        <v>0.01000013317742114</v>
+        <v>0.01</v>
       </c>
       <c r="J69">
-        <v>20741981.90976076</v>
+        <v>20741981.91</v>
       </c>
       <c r="K69">
-        <v>61759.79257984829</v>
+        <v>61759.793</v>
       </c>
       <c r="L69">
-        <v>15141646.79412536</v>
+        <v>15141646.794</v>
       </c>
       <c r="M69">
-        <v>11038831.42125</v>
+        <v>11038831.421</v>
       </c>
       <c r="N69">
-        <v>1.371671168469639</v>
+        <v>1.372</v>
       </c>
     </row>
     <row r="70">
@@ -14714,40 +14714,40 @@
         <v>0</v>
       </c>
       <c r="C70">
-        <v>346.0774139495549</v>
+        <v>346.077</v>
       </c>
       <c r="D70">
-        <v>60972196.5612449</v>
+        <v>60972196.561</v>
       </c>
       <c r="E70">
-        <v>37933.76897166931</v>
+        <v>37933.769</v>
       </c>
       <c r="F70">
-        <v>0.01954857176713309</v>
+        <v>0.02</v>
       </c>
       <c r="G70">
-        <v>4872414.507034959</v>
+        <v>4872414.507</v>
       </c>
       <c r="H70">
         <v>15412938.72</v>
       </c>
       <c r="I70">
-        <v>0.01000008148205674</v>
+        <v>0.01</v>
       </c>
       <c r="J70">
-        <v>21791494.01037378</v>
+        <v>21791494.01</v>
       </c>
       <c r="K70">
-        <v>62967.10831741871</v>
+        <v>62967.108</v>
       </c>
       <c r="L70">
-        <v>15907790.62757286</v>
+        <v>15907790.628</v>
       </c>
       <c r="M70">
         <v>11559704.04</v>
       </c>
       <c r="N70">
-        <v>1.37614168775664</v>
+        <v>1.376</v>
       </c>
     </row>
     <row r="71">
@@ -14758,40 +14758,40 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <v>356.6170403032269</v>
+        <v>356.617</v>
       </c>
       <c r="D71">
-        <v>63981182.20138855</v>
+        <v>63981182.201</v>
       </c>
       <c r="E71">
-        <v>38700.0819371624</v>
+        <v>38700.082</v>
       </c>
       <c r="F71">
-        <v>0.01958577831536346</v>
+        <v>0.02</v>
       </c>
       <c r="G71">
-        <v>5113347.806961036</v>
+        <v>5113347.807</v>
       </c>
       <c r="H71">
         <v>16143417.187</v>
       </c>
       <c r="I71">
-        <v>0.01000005596449981</v>
+        <v>0.01</v>
       </c>
       <c r="J71">
-        <v>22894945.27320727</v>
+        <v>22894945.273</v>
       </c>
       <c r="K71">
-        <v>64200.36814208315</v>
+        <v>64200.368</v>
       </c>
       <c r="L71">
-        <v>16713310.04944131</v>
+        <v>16713310.049</v>
       </c>
       <c r="M71">
-        <v>12107562.89025</v>
+        <v>12107562.89</v>
       </c>
       <c r="N71">
-        <v>1.380402497260636</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="72">
@@ -14802,40 +14802,40 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>367.4776460655443</v>
+        <v>367.478</v>
       </c>
       <c r="D72">
-        <v>67145671.23163481</v>
+        <v>67145671.23199999</v>
       </c>
       <c r="E72">
-        <v>39481.87545143832</v>
+        <v>39481.875</v>
       </c>
       <c r="F72">
-        <v>0.01962090531198209</v>
+        <v>0.02</v>
       </c>
       <c r="G72">
-        <v>5366712.80014674</v>
+        <v>5366712.8</v>
       </c>
       <c r="H72">
         <v>16911731.07</v>
       </c>
       <c r="I72">
-        <v>0.01000003797562236</v>
+        <v>0.01</v>
       </c>
       <c r="J72">
-        <v>24055100.48686212</v>
+        <v>24055100.487</v>
       </c>
       <c r="K72">
-        <v>65460.03748639335</v>
+        <v>65460.037</v>
       </c>
       <c r="L72">
-        <v>17560223.35540935</v>
+        <v>17560223.355</v>
       </c>
       <c r="M72">
-        <v>12683798.3025</v>
+        <v>12683798.303</v>
       </c>
       <c r="N72">
-        <v>1.384460942740488</v>
+        <v>1.384</v>
       </c>
     </row>
     <row r="73">
@@ -14846,40 +14846,40 @@
         <v>1</v>
       </c>
       <c r="C73">
-        <v>378.6690065148058</v>
+        <v>378.669</v>
       </c>
       <c r="D73">
-        <v>70473619.50408495</v>
+        <v>70473619.50399999</v>
       </c>
       <c r="E73">
-        <v>39876.66659479363</v>
+        <v>39876.667</v>
       </c>
       <c r="F73">
-        <v>0.01281104219742135</v>
+        <v>0.013</v>
       </c>
       <c r="G73">
-        <v>5633146.297878113</v>
+        <v>5633146.298</v>
       </c>
       <c r="H73">
         <v>17121205.076</v>
       </c>
       <c r="I73">
-        <v>0.01000002544994114</v>
+        <v>0.01</v>
       </c>
       <c r="J73">
-        <v>25105243.47015783</v>
+        <v>25105243.47</v>
       </c>
       <c r="K73">
-        <v>66298.64878887632</v>
+        <v>66298.649</v>
       </c>
       <c r="L73">
-        <v>18326827.73321522</v>
+        <v>18326827.733</v>
       </c>
       <c r="M73">
         <v>12840903.807</v>
       </c>
       <c r="N73">
-        <v>1.427222570051857</v>
+        <v>1.427</v>
       </c>
     </row>
     <row r="74">
@@ -14890,40 +14890,40 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>390.2011946308555</v>
+        <v>390.201</v>
       </c>
       <c r="D74">
-        <v>73930985.591461</v>
+        <v>73930985.59100001</v>
       </c>
       <c r="E74">
-        <v>40682.22869580863</v>
+        <v>40682.229</v>
       </c>
       <c r="F74">
-        <v>0.01949242637070605</v>
+        <v>0.019</v>
       </c>
       <c r="G74">
-        <v>5909925.315366144</v>
+        <v>5909925.315</v>
       </c>
       <c r="H74">
         <v>17926792.249</v>
       </c>
       <c r="I74">
-        <v>0.01000001464179521</v>
+        <v>0.01</v>
       </c>
       <c r="J74">
-        <v>26374077.36468208</v>
+        <v>26374077.365</v>
       </c>
       <c r="K74">
-        <v>67590.97031887079</v>
+        <v>67590.97</v>
       </c>
       <c r="L74">
-        <v>19253076.47621792</v>
+        <v>19253076.476</v>
       </c>
       <c r="M74">
-        <v>13445094.18675</v>
+        <v>13445094.187</v>
       </c>
       <c r="N74">
-        <v>1.431977806090166</v>
+        <v>1.432</v>
       </c>
     </row>
     <row r="75">
@@ -14934,40 +14934,40 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <v>402.0845901614437</v>
+        <v>402.085</v>
       </c>
       <c r="D75">
-        <v>77567265.50897308</v>
+        <v>77567265.509</v>
       </c>
       <c r="E75">
-        <v>41504.06423073891</v>
+        <v>41504.064</v>
       </c>
       <c r="F75">
-        <v>0.01953276156905556</v>
+        <v>0.02</v>
       </c>
       <c r="G75">
-        <v>6201009.85004514</v>
+        <v>6201009.85</v>
       </c>
       <c r="H75">
         <v>18774123.321</v>
       </c>
       <c r="I75">
-        <v>0.01000000960071952</v>
+        <v>0.01</v>
       </c>
       <c r="J75">
-        <v>27708135.07804781</v>
+        <v>27708135.078</v>
       </c>
       <c r="K75">
-        <v>68911.20862633041</v>
+        <v>68911.209</v>
       </c>
       <c r="L75">
-        <v>20226938.6069749</v>
+        <v>20226938.607</v>
       </c>
       <c r="M75">
-        <v>14080592.49075</v>
+        <v>14080592.491</v>
       </c>
       <c r="N75">
-        <v>1.43651189538101</v>
+        <v>1.437</v>
       </c>
     </row>
     <row r="76">
@@ -14978,40 +14978,40 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>414.3298889647012</v>
+        <v>414.33</v>
       </c>
       <c r="D76">
-        <v>81391608.6581261</v>
+        <v>81391608.65800001</v>
       </c>
       <c r="E76">
-        <v>42342.50194475638</v>
+        <v>42342.502</v>
       </c>
       <c r="F76">
-        <v>0.0195708502737916</v>
+        <v>0.02</v>
       </c>
       <c r="G76">
-        <v>6507132.157604291</v>
+        <v>6507132.158</v>
       </c>
       <c r="H76">
         <v>19665349.8</v>
       </c>
       <c r="I76">
-        <v>0.01000000620955301</v>
+        <v>0.01</v>
       </c>
       <c r="J76">
-        <v>29110759.81536696</v>
+        <v>29110759.815</v>
       </c>
       <c r="K76">
-        <v>70259.85957254234</v>
+        <v>70259.86</v>
       </c>
       <c r="L76">
-        <v>21250854.66521788</v>
+        <v>21250854.665</v>
       </c>
       <c r="M76">
         <v>14749012.35</v>
       </c>
       <c r="N76">
-        <v>1.440832386666072</v>
+        <v>1.441</v>
       </c>
     </row>
     <row r="77">
@@ -15022,40 +15022,40 @@
         <v>0</v>
       </c>
       <c r="C77">
-        <v>426.9481126361337</v>
+        <v>426.948</v>
       </c>
       <c r="D77">
-        <v>85413634.26564281</v>
+        <v>85413634.266</v>
       </c>
       <c r="E77">
-        <v>43197.87722412597</v>
+        <v>43197.877</v>
       </c>
       <c r="F77">
-        <v>0.01960681222825407</v>
+        <v>0.02</v>
       </c>
       <c r="G77">
-        <v>6829062.067607459</v>
+        <v>6829062.068</v>
       </c>
       <c r="H77">
         <v>20602732.638</v>
       </c>
       <c r="I77">
-        <v>0.0100000039599856</v>
+        <v>0.01</v>
       </c>
       <c r="J77">
-        <v>30585466.15012581</v>
+        <v>30585466.15</v>
       </c>
       <c r="K77">
-        <v>71637.43144636467</v>
+        <v>71637.431</v>
       </c>
       <c r="L77">
-        <v>22327390.28959184</v>
+        <v>22327390.29</v>
       </c>
       <c r="M77">
-        <v>15452049.4785</v>
+        <v>15452049.479</v>
       </c>
       <c r="N77">
-        <v>1.444946854503553</v>
+        <v>1.445</v>
       </c>
     </row>
     <row r="78">
@@ -15066,40 +15066,40 @@
         <v>1</v>
       </c>
       <c r="C78">
-        <v>439.9506184288007</v>
+        <v>439.951</v>
       </c>
       <c r="D78">
-        <v>89643455.43254854</v>
+        <v>89643455.433</v>
       </c>
       <c r="E78">
-        <v>43629.82679836868</v>
+        <v>43629.827</v>
       </c>
       <c r="F78">
-        <v>0.0127978441892726</v>
+        <v>0.013</v>
       </c>
       <c r="G78">
-        <v>7167608.907905676</v>
+        <v>7167608.908</v>
       </c>
       <c r="H78">
         <v>20859325.364</v>
       </c>
       <c r="I78">
-        <v>0.01000000248901587</v>
+        <v>0.01</v>
       </c>
       <c r="J78">
-        <v>31920281.055962</v>
+        <v>31920281.056</v>
       </c>
       <c r="K78">
-        <v>72554.23613213495</v>
+        <v>72554.236</v>
       </c>
       <c r="L78">
-        <v>23301805.17085226</v>
+        <v>23301805.171</v>
       </c>
       <c r="M78">
         <v>15644494.023</v>
       </c>
       <c r="N78">
-        <v>1.489457258035622</v>
+        <v>1.489</v>
       </c>
     </row>
     <row r="79">
@@ -15110,40 +15110,40 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <v>453.3491094756114</v>
+        <v>453.349</v>
       </c>
       <c r="D79">
-        <v>94037787.4792371</v>
+        <v>94037787.479</v>
       </c>
       <c r="E79">
-        <v>44511.20776483099</v>
+        <v>44511.208</v>
       </c>
       <c r="F79">
-        <v>0.01947995063527064</v>
+        <v>0.019</v>
       </c>
       <c r="G79">
-        <v>7519310.172708689</v>
+        <v>7519310.173</v>
       </c>
       <c r="H79">
         <v>21842154.019</v>
       </c>
       <c r="I79">
-        <v>0.01000000131003753</v>
+        <v>0.01</v>
       </c>
       <c r="J79">
-        <v>33533140.63510962</v>
+        <v>33533140.635</v>
       </c>
       <c r="K79">
-        <v>73967.5890703687</v>
+        <v>73967.58900000001</v>
       </c>
       <c r="L79">
-        <v>24479192.66363002</v>
+        <v>24479192.664</v>
       </c>
       <c r="M79">
-        <v>16381615.51425</v>
+        <v>16381615.514</v>
       </c>
       <c r="N79">
-        <v>1.49430882701014</v>
+        <v>1.494</v>
       </c>
     </row>
     <row r="80">
@@ -15154,40 +15154,40 @@
         <v>1</v>
       </c>
       <c r="C80">
-        <v>467.1556453229329</v>
+        <v>467.156</v>
       </c>
       <c r="D80">
-        <v>98659561.13884501</v>
+        <v>98659561.139</v>
       </c>
       <c r="E80">
-        <v>44956.2898333569</v>
+        <v>44956.29</v>
       </c>
       <c r="F80">
-        <v>0.01267886731376725</v>
+        <v>0.013</v>
       </c>
       <c r="G80">
-        <v>7889200.578502534</v>
+        <v>7889200.579</v>
       </c>
       <c r="H80">
         <v>22103097.386</v>
       </c>
       <c r="I80">
-        <v>0.01000000080277032</v>
+        <v>0.01</v>
       </c>
       <c r="J80">
-        <v>34992487.16377202</v>
+        <v>34992487.164</v>
       </c>
       <c r="K80">
-        <v>74905.41431771117</v>
+        <v>74905.414</v>
       </c>
       <c r="L80">
-        <v>25544515.62955357</v>
+        <v>25544515.63</v>
       </c>
       <c r="M80">
-        <v>16577323.0395</v>
+        <v>16577323.04</v>
       </c>
       <c r="N80">
-        <v>1.540931281165649</v>
+        <v>1.541</v>
       </c>
     </row>
     <row r="81">
@@ -15198,40 +15198,40 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <v>481.3826527849974</v>
+        <v>481.383</v>
       </c>
       <c r="D81">
-        <v>103461300.4842342</v>
+        <v>103461300.484</v>
       </c>
       <c r="E81">
-        <v>45864.46713062192</v>
+        <v>45864.467</v>
       </c>
       <c r="F81">
-        <v>0.01936758536284223</v>
+        <v>0.019</v>
       </c>
       <c r="G81">
-        <v>8273482.298637872</v>
+        <v>8273482.299</v>
       </c>
       <c r="H81">
         <v>23133799.207</v>
       </c>
       <c r="I81">
-        <v>0.01000000040697558</v>
+        <v>0.01</v>
       </c>
       <c r="J81">
-        <v>36756526.68063061</v>
+        <v>36756526.681</v>
       </c>
       <c r="K81">
-        <v>76356.1513236485</v>
+        <v>76356.151</v>
       </c>
       <c r="L81">
-        <v>26832264.47686034</v>
+        <v>26832264.477</v>
       </c>
       <c r="M81">
-        <v>17350349.40525</v>
+        <v>17350349.405</v>
       </c>
       <c r="N81">
-        <v>1.546497067588808</v>
+        <v>1.546</v>
       </c>
     </row>
     <row r="82">
@@ -15242,40 +15242,40 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>496.042937128872</v>
+        <v>496.043</v>
       </c>
       <c r="D82">
-        <v>108511980.1350225</v>
+        <v>108511980.135</v>
       </c>
       <c r="E82">
-        <v>46790.99082627358</v>
+        <v>46790.991</v>
       </c>
       <c r="F82">
-        <v>0.01941483652378191</v>
+        <v>0.019</v>
       </c>
       <c r="G82">
-        <v>8677673.540304968</v>
+        <v>8677673.539999999</v>
       </c>
       <c r="H82">
         <v>24217932.518</v>
       </c>
       <c r="I82">
-        <v>0.01000000024271589</v>
+        <v>0.01</v>
       </c>
       <c r="J82">
-        <v>38611284.55123557</v>
+        <v>38611284.551</v>
       </c>
       <c r="K82">
-        <v>77838.59351918229</v>
+        <v>77838.594</v>
       </c>
       <c r="L82">
-        <v>28186237.72240197</v>
+        <v>28186237.722</v>
       </c>
       <c r="M82">
-        <v>18163449.3885</v>
+        <v>18163449.388</v>
       </c>
       <c r="N82">
-        <v>1.551810843828364</v>
+        <v>1.552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>